<commit_message>
primeiros testes - conta
</commit_message>
<xml_diff>
--- a/app_moneytracker/relatorios/Relatory - Test Case Specification and Report.xlsx
+++ b/app_moneytracker/relatorios/Relatory - Test Case Specification and Report.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="516" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="516" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Requisitos" sheetId="5" r:id="rId1"/>
@@ -749,7 +749,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -1228,30 +1228,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1297,6 +1273,30 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1304,6 +1304,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1326,12 +1332,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1920,14 +1920,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
@@ -1937,9 +1937,9 @@
       <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:6" ht="15">
       <c r="B25" s="34"/>
       <c r="C25" s="50"/>
       <c r="D25" s="50"/>
@@ -1951,73 +1951,74 @@
     <mergeCell ref="C25:F25"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:F121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C124" sqref="C124"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="10.3984375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.8984375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.296875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="25.69921875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.25" style="2" customWidth="1"/>
+    <col min="4" max="4" width="25.75" style="2" customWidth="1"/>
     <col min="5" max="5" width="41" style="2" customWidth="1"/>
-    <col min="6" max="6" width="29.09765625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.796875" style="8"/>
+    <col min="6" max="6" width="29.125" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.75" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.6" customHeight="1" thickBot="1">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="63"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="55"/>
     </row>
     <row r="2" spans="1:6" ht="15.6" customHeight="1" thickBot="1">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="51" t="s">
+      <c r="B2" s="65"/>
+      <c r="C2" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="53"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="68"/>
     </row>
     <row r="3" spans="1:6" customFormat="1" ht="15.6" customHeight="1" thickBot="1"/>
     <row r="4" spans="1:6" ht="18.600000000000001" customHeight="1" thickBot="1">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="55"/>
-      <c r="C4" s="56"/>
-    </row>
-    <row r="5" spans="1:6" ht="17.399999999999999" customHeight="1">
+      <c r="B4" s="70"/>
+      <c r="C4" s="71"/>
+    </row>
+    <row r="5" spans="1:6" ht="17.45" customHeight="1">
       <c r="A5" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="64" t="s">
+      <c r="B5" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="67"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="59"/>
     </row>
     <row r="6" spans="1:6">
       <c r="B6" s="10" t="s">
@@ -2053,17 +2054,17 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.8" customHeight="1">
+    <row r="9" spans="1:6" ht="13.9" customHeight="1">
       <c r="A9" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="68" t="s">
+      <c r="B9" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="70"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="62"/>
     </row>
     <row r="10" spans="1:6">
       <c r="B10" s="10" t="s">
@@ -2082,7 +2083,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="39.6">
+    <row r="11" spans="1:6" ht="38.25">
       <c r="B11" s="6" t="s">
         <v>24</v>
       </c>
@@ -2103,17 +2104,17 @@
       <c r="E12" s="1"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" ht="13.8" customHeight="1">
+    <row r="13" spans="1:6" ht="13.9" customHeight="1">
       <c r="A13" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="71" t="s">
+      <c r="B13" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="67"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="59"/>
     </row>
     <row r="14" spans="1:6">
       <c r="B14" s="10" t="s">
@@ -2132,7 +2133,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="52.8">
+    <row r="15" spans="1:6" ht="51">
       <c r="B15" s="6" t="s">
         <v>25</v>
       </c>
@@ -2149,17 +2150,17 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.8" customHeight="1">
+    <row r="17" spans="1:6" ht="13.9" customHeight="1">
       <c r="A17" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="59" t="s">
+      <c r="B17" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="59"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
     </row>
     <row r="18" spans="1:6">
       <c r="B18" s="10" t="s">
@@ -2178,7 +2179,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="39.6">
+    <row r="19" spans="1:6" ht="38.25">
       <c r="B19" s="6" t="s">
         <v>26</v>
       </c>
@@ -2195,17 +2196,17 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="22.2" customHeight="1">
+    <row r="21" spans="1:6" ht="22.15" customHeight="1">
       <c r="A21" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="71" t="s">
+      <c r="B21" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="69"/>
-      <c r="D21" s="69"/>
-      <c r="E21" s="69"/>
-      <c r="F21" s="70"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="62"/>
     </row>
     <row r="22" spans="1:6">
       <c r="B22" s="10" t="s">
@@ -2224,7 +2225,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="39.6">
+    <row r="23" spans="1:6" ht="38.25">
       <c r="B23" s="4" t="s">
         <v>28</v>
       </c>
@@ -2241,17 +2242,17 @@
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="13.8" customHeight="1">
+    <row r="25" spans="1:6" ht="13.9" customHeight="1">
       <c r="A25" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="59" t="s">
+      <c r="B25" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="59"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="51"/>
     </row>
     <row r="26" spans="1:6">
       <c r="B26" s="10" t="s">
@@ -2270,7 +2271,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="39.6">
+    <row r="27" spans="1:6" ht="38.25">
       <c r="B27" s="4" t="s">
         <v>30</v>
       </c>
@@ -2294,17 +2295,17 @@
       <c r="E28" s="38"/>
       <c r="F28" s="38"/>
     </row>
-    <row r="29" spans="1:6" ht="13.8" customHeight="1">
+    <row r="29" spans="1:6" ht="13.9" customHeight="1">
       <c r="A29" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="59" t="s">
+      <c r="B29" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="59"/>
-      <c r="D29" s="59"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="59"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
     </row>
     <row r="30" spans="1:6">
       <c r="B30" s="10" t="s">
@@ -2323,7 +2324,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="39.6">
+    <row r="31" spans="1:6" ht="38.25">
       <c r="B31" s="4" t="s">
         <v>39</v>
       </c>
@@ -2351,13 +2352,13 @@
       <c r="A33" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B33" s="59" t="s">
+      <c r="B33" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="59"/>
-      <c r="D33" s="59"/>
-      <c r="E33" s="59"/>
-      <c r="F33" s="59"/>
+      <c r="C33" s="51"/>
+      <c r="D33" s="51"/>
+      <c r="E33" s="51"/>
+      <c r="F33" s="51"/>
     </row>
     <row r="34" spans="1:6">
       <c r="B34" s="10" t="s">
@@ -2376,7 +2377,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="39.6">
+    <row r="35" spans="1:6" ht="38.25">
       <c r="B35" s="4" t="s">
         <v>49</v>
       </c>
@@ -2404,13 +2405,13 @@
       <c r="A37" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="59" t="s">
+      <c r="B37" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="C37" s="59"/>
-      <c r="D37" s="59"/>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="51"/>
+      <c r="F37" s="51"/>
     </row>
     <row r="38" spans="1:6">
       <c r="B38" s="10" t="s">
@@ -2429,7 +2430,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="40.799999999999997" customHeight="1">
+    <row r="39" spans="1:6" ht="40.9" customHeight="1">
       <c r="B39" s="4" t="s">
         <v>52</v>
       </c>
@@ -2457,11 +2458,11 @@
       <c r="A41" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B41" s="59"/>
-      <c r="C41" s="59"/>
-      <c r="D41" s="59"/>
-      <c r="E41" s="59"/>
-      <c r="F41" s="59"/>
+      <c r="B41" s="51"/>
+      <c r="C41" s="51"/>
+      <c r="D41" s="51"/>
+      <c r="E41" s="51"/>
+      <c r="F41" s="51"/>
     </row>
     <row r="42" spans="1:6">
       <c r="B42" s="10" t="s">
@@ -2489,31 +2490,31 @@
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
     </row>
-    <row r="44" spans="1:6" ht="13.8" thickBot="1">
+    <row r="44" spans="1:6" ht="13.5" thickBot="1">
       <c r="B44" s="37"/>
       <c r="C44" s="37"/>
       <c r="D44" s="37"/>
       <c r="E44" s="38"/>
       <c r="F44" s="38"/>
     </row>
-    <row r="45" spans="1:6" ht="13.8" customHeight="1" thickBot="1">
-      <c r="A45" s="54" t="s">
+    <row r="45" spans="1:6" ht="13.9" customHeight="1" thickBot="1">
+      <c r="A45" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="57"/>
-      <c r="C45" s="58"/>
-    </row>
-    <row r="46" spans="1:6" ht="16.2" customHeight="1">
+      <c r="B45" s="72"/>
+      <c r="C45" s="73"/>
+    </row>
+    <row r="46" spans="1:6" ht="16.149999999999999" customHeight="1">
       <c r="A46" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B46" s="59" t="s">
+      <c r="B46" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="C46" s="59"/>
-      <c r="D46" s="59"/>
-      <c r="E46" s="59"/>
-      <c r="F46" s="59"/>
+      <c r="C46" s="51"/>
+      <c r="D46" s="51"/>
+      <c r="E46" s="51"/>
+      <c r="F46" s="51"/>
     </row>
     <row r="47" spans="1:6">
       <c r="B47" s="10" t="s">
@@ -2532,7 +2533,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="66">
+    <row r="48" spans="1:6" ht="63.75">
       <c r="B48" s="4" t="s">
         <v>34</v>
       </c>
@@ -2549,17 +2550,17 @@
         <v>129</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="13.8" customHeight="1">
+    <row r="50" spans="1:6" ht="13.9" customHeight="1">
       <c r="A50" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B50" s="59" t="s">
+      <c r="B50" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="C50" s="59"/>
-      <c r="D50" s="59"/>
-      <c r="E50" s="59"/>
-      <c r="F50" s="59"/>
+      <c r="C50" s="51"/>
+      <c r="D50" s="51"/>
+      <c r="E50" s="51"/>
+      <c r="F50" s="51"/>
     </row>
     <row r="51" spans="1:6">
       <c r="B51" s="10" t="s">
@@ -2578,7 +2579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="39.6">
+    <row r="52" spans="1:6" ht="38.25">
       <c r="B52" s="4" t="s">
         <v>35</v>
       </c>
@@ -2595,17 +2596,17 @@
         <v>132</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="13.8" customHeight="1">
+    <row r="54" spans="1:6" ht="13.9" customHeight="1">
       <c r="A54" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B54" s="59" t="s">
+      <c r="B54" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="C54" s="59"/>
-      <c r="D54" s="59"/>
-      <c r="E54" s="59"/>
-      <c r="F54" s="59"/>
+      <c r="C54" s="51"/>
+      <c r="D54" s="51"/>
+      <c r="E54" s="51"/>
+      <c r="F54" s="51"/>
     </row>
     <row r="55" spans="1:6">
       <c r="B55" s="10" t="s">
@@ -2624,7 +2625,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="39.6">
+    <row r="56" spans="1:6" ht="38.25">
       <c r="B56" s="4" t="s">
         <v>36</v>
       </c>
@@ -2641,17 +2642,17 @@
         <v>134</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="13.8" customHeight="1">
+    <row r="58" spans="1:6" ht="13.9" customHeight="1">
       <c r="A58" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B58" s="59" t="s">
+      <c r="B58" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="C58" s="59"/>
-      <c r="D58" s="59"/>
-      <c r="E58" s="59"/>
-      <c r="F58" s="59"/>
+      <c r="C58" s="51"/>
+      <c r="D58" s="51"/>
+      <c r="E58" s="51"/>
+      <c r="F58" s="51"/>
     </row>
     <row r="59" spans="1:6">
       <c r="B59" s="10" t="s">
@@ -2670,7 +2671,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="66">
+    <row r="60" spans="1:6" ht="63.75">
       <c r="B60" s="4" t="s">
         <v>37</v>
       </c>
@@ -2687,17 +2688,17 @@
         <v>55</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="13.8" customHeight="1">
+    <row r="62" spans="1:6" ht="13.9" customHeight="1">
       <c r="A62" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B62" s="59" t="s">
+      <c r="B62" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="C62" s="59"/>
-      <c r="D62" s="59"/>
-      <c r="E62" s="59"/>
-      <c r="F62" s="59"/>
+      <c r="C62" s="51"/>
+      <c r="D62" s="51"/>
+      <c r="E62" s="51"/>
+      <c r="F62" s="51"/>
     </row>
     <row r="63" spans="1:6">
       <c r="B63" s="10" t="s">
@@ -2716,7 +2717,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="39.6">
+    <row r="64" spans="1:6" ht="38.25">
       <c r="B64" s="4" t="s">
         <v>53</v>
       </c>
@@ -2733,17 +2734,17 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="13.8" customHeight="1">
+    <row r="66" spans="1:6" ht="13.9" customHeight="1">
       <c r="A66" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B66" s="59" t="s">
+      <c r="B66" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="C66" s="59"/>
-      <c r="D66" s="59"/>
-      <c r="E66" s="59"/>
-      <c r="F66" s="59"/>
+      <c r="C66" s="51"/>
+      <c r="D66" s="51"/>
+      <c r="E66" s="51"/>
+      <c r="F66" s="51"/>
     </row>
     <row r="67" spans="1:6">
       <c r="B67" s="10" t="s">
@@ -2762,7 +2763,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="52.8">
+    <row r="68" spans="1:6" ht="51">
       <c r="B68" s="4" t="s">
         <v>56</v>
       </c>
@@ -2779,17 +2780,17 @@
         <v>66</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="13.8" customHeight="1">
+    <row r="70" spans="1:6" ht="13.9" customHeight="1">
       <c r="A70" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B70" s="59" t="s">
+      <c r="B70" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="C70" s="59"/>
-      <c r="D70" s="59"/>
-      <c r="E70" s="59"/>
-      <c r="F70" s="59"/>
+      <c r="C70" s="51"/>
+      <c r="D70" s="51"/>
+      <c r="E70" s="51"/>
+      <c r="F70" s="51"/>
     </row>
     <row r="71" spans="1:6">
       <c r="B71" s="10" t="s">
@@ -2808,7 +2809,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="39.6">
+    <row r="72" spans="1:6" ht="38.25">
       <c r="B72" s="4" t="s">
         <v>62</v>
       </c>
@@ -2825,17 +2826,17 @@
         <v>70</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="13.8" customHeight="1">
+    <row r="74" spans="1:6" ht="13.9" customHeight="1">
       <c r="A74" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B74" s="59" t="s">
+      <c r="B74" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="C74" s="59"/>
-      <c r="D74" s="59"/>
-      <c r="E74" s="59"/>
-      <c r="F74" s="59"/>
+      <c r="C74" s="51"/>
+      <c r="D74" s="51"/>
+      <c r="E74" s="51"/>
+      <c r="F74" s="51"/>
     </row>
     <row r="75" spans="1:6">
       <c r="B75" s="10" t="s">
@@ -2854,7 +2855,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="39.6">
+    <row r="76" spans="1:6" ht="38.25">
       <c r="B76" s="4" t="s">
         <v>64</v>
       </c>
@@ -2871,17 +2872,17 @@
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="13.8" customHeight="1">
+    <row r="78" spans="1:6" ht="13.9" customHeight="1">
       <c r="A78" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B78" s="59" t="s">
+      <c r="B78" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="C78" s="59"/>
-      <c r="D78" s="59"/>
-      <c r="E78" s="59"/>
-      <c r="F78" s="59"/>
+      <c r="C78" s="51"/>
+      <c r="D78" s="51"/>
+      <c r="E78" s="51"/>
+      <c r="F78" s="51"/>
     </row>
     <row r="79" spans="1:6">
       <c r="B79" s="10" t="s">
@@ -2900,7 +2901,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="52.8">
+    <row r="80" spans="1:6" ht="51">
       <c r="B80" s="4" t="s">
         <v>67</v>
       </c>
@@ -2917,17 +2918,17 @@
         <v>74</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="13.8" customHeight="1">
+    <row r="82" spans="1:6" ht="13.9" customHeight="1">
       <c r="A82" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B82" s="59" t="s">
+      <c r="B82" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="C82" s="59"/>
-      <c r="D82" s="59"/>
-      <c r="E82" s="59"/>
-      <c r="F82" s="59"/>
+      <c r="C82" s="51"/>
+      <c r="D82" s="51"/>
+      <c r="E82" s="51"/>
+      <c r="F82" s="51"/>
     </row>
     <row r="83" spans="1:6">
       <c r="B83" s="10" t="s">
@@ -2946,7 +2947,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="39.6">
+    <row r="84" spans="1:6" ht="38.25">
       <c r="B84" s="4" t="s">
         <v>68</v>
       </c>
@@ -2963,17 +2964,17 @@
         <v>81</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="13.8" customHeight="1">
+    <row r="86" spans="1:6" ht="13.9" customHeight="1">
       <c r="A86" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B86" s="59" t="s">
+      <c r="B86" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="C86" s="59"/>
-      <c r="D86" s="59"/>
-      <c r="E86" s="59"/>
-      <c r="F86" s="59"/>
+      <c r="C86" s="51"/>
+      <c r="D86" s="51"/>
+      <c r="E86" s="51"/>
+      <c r="F86" s="51"/>
     </row>
     <row r="87" spans="1:6">
       <c r="B87" s="10" t="s">
@@ -2992,7 +2993,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="39.6">
+    <row r="88" spans="1:6" ht="38.25">
       <c r="B88" s="4" t="s">
         <v>71</v>
       </c>
@@ -3009,17 +3010,17 @@
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="13.8" customHeight="1">
+    <row r="90" spans="1:6" ht="13.9" customHeight="1">
       <c r="A90" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B90" s="59" t="s">
+      <c r="B90" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="C90" s="59"/>
-      <c r="D90" s="59"/>
-      <c r="E90" s="59"/>
-      <c r="F90" s="59"/>
+      <c r="C90" s="51"/>
+      <c r="D90" s="51"/>
+      <c r="E90" s="51"/>
+      <c r="F90" s="51"/>
     </row>
     <row r="91" spans="1:6">
       <c r="B91" s="10" t="s">
@@ -3038,7 +3039,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="39.6">
+    <row r="92" spans="1:6" ht="38.25">
       <c r="B92" s="4" t="s">
         <v>72</v>
       </c>
@@ -3055,7 +3056,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="41.4" customHeight="1">
+    <row r="93" spans="1:6" ht="41.45" customHeight="1">
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
       <c r="D93" s="4" t="s">
@@ -3068,17 +3069,17 @@
         <v>91</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="13.8" customHeight="1">
+    <row r="95" spans="1:6" ht="13.9" customHeight="1">
       <c r="A95" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B95" s="59" t="s">
+      <c r="B95" s="51" t="s">
         <v>93</v>
       </c>
-      <c r="C95" s="59"/>
-      <c r="D95" s="59"/>
-      <c r="E95" s="59"/>
-      <c r="F95" s="59"/>
+      <c r="C95" s="51"/>
+      <c r="D95" s="51"/>
+      <c r="E95" s="51"/>
+      <c r="F95" s="51"/>
     </row>
     <row r="96" spans="1:6">
       <c r="B96" s="10" t="s">
@@ -3097,7 +3098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="39.6">
+    <row r="97" spans="1:6" ht="38.25">
       <c r="B97" s="4" t="s">
         <v>75</v>
       </c>
@@ -3114,17 +3115,17 @@
         <v>95</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="13.8" customHeight="1">
+    <row r="99" spans="1:6" ht="13.9" customHeight="1">
       <c r="A99" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B99" s="59" t="s">
+      <c r="B99" s="51" t="s">
         <v>99</v>
       </c>
-      <c r="C99" s="59"/>
-      <c r="D99" s="59"/>
-      <c r="E99" s="59"/>
-      <c r="F99" s="59"/>
+      <c r="C99" s="51"/>
+      <c r="D99" s="51"/>
+      <c r="E99" s="51"/>
+      <c r="F99" s="51"/>
     </row>
     <row r="100" spans="1:6">
       <c r="B100" s="10" t="s">
@@ -3143,7 +3144,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="52.8">
+    <row r="101" spans="1:6" ht="51">
       <c r="B101" s="4" t="s">
         <v>77</v>
       </c>
@@ -3160,17 +3161,17 @@
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="13.8" customHeight="1">
+    <row r="103" spans="1:6" ht="13.9" customHeight="1">
       <c r="A103" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B103" s="59" t="s">
+      <c r="B103" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="C103" s="59"/>
-      <c r="D103" s="59"/>
-      <c r="E103" s="59"/>
-      <c r="F103" s="59"/>
+      <c r="C103" s="51"/>
+      <c r="D103" s="51"/>
+      <c r="E103" s="51"/>
+      <c r="F103" s="51"/>
     </row>
     <row r="104" spans="1:6">
       <c r="B104" s="10" t="s">
@@ -3189,7 +3190,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="66">
+    <row r="105" spans="1:6" ht="63.75">
       <c r="B105" s="4" t="s">
         <v>78</v>
       </c>
@@ -3206,17 +3207,17 @@
         <v>101</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="13.8" customHeight="1">
+    <row r="107" spans="1:6" ht="13.9" customHeight="1">
       <c r="A107" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B107" s="59" t="s">
+      <c r="B107" s="51" t="s">
         <v>104</v>
       </c>
-      <c r="C107" s="59"/>
-      <c r="D107" s="59"/>
-      <c r="E107" s="59"/>
-      <c r="F107" s="59"/>
+      <c r="C107" s="51"/>
+      <c r="D107" s="51"/>
+      <c r="E107" s="51"/>
+      <c r="F107" s="51"/>
     </row>
     <row r="108" spans="1:6">
       <c r="B108" s="10" t="s">
@@ -3235,7 +3236,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="66">
+    <row r="109" spans="1:6" ht="63.75">
       <c r="B109" s="4" t="s">
         <v>86</v>
       </c>
@@ -3252,17 +3253,17 @@
         <v>106</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="13.8" customHeight="1">
+    <row r="111" spans="1:6" ht="13.9" customHeight="1">
       <c r="A111" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B111" s="59" t="s">
+      <c r="B111" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="C111" s="59"/>
-      <c r="D111" s="59"/>
-      <c r="E111" s="59"/>
-      <c r="F111" s="59"/>
+      <c r="C111" s="51"/>
+      <c r="D111" s="51"/>
+      <c r="E111" s="51"/>
+      <c r="F111" s="51"/>
     </row>
     <row r="112" spans="1:6">
       <c r="B112" s="10" t="s">
@@ -3281,7 +3282,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="26.4">
+    <row r="113" spans="1:6" ht="25.5">
       <c r="B113" s="4" t="s">
         <v>92</v>
       </c>
@@ -3298,17 +3299,17 @@
         <v>109</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="13.8" customHeight="1">
+    <row r="115" spans="1:6" ht="13.9" customHeight="1">
       <c r="A115" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B115" s="59" t="s">
+      <c r="B115" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="C115" s="59"/>
-      <c r="D115" s="59"/>
-      <c r="E115" s="59"/>
-      <c r="F115" s="59"/>
+      <c r="C115" s="51"/>
+      <c r="D115" s="51"/>
+      <c r="E115" s="51"/>
+      <c r="F115" s="51"/>
     </row>
     <row r="116" spans="1:6">
       <c r="B116" s="10" t="s">
@@ -3327,7 +3328,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="39.6">
+    <row r="117" spans="1:6" ht="38.25">
       <c r="B117" s="4" t="s">
         <v>107</v>
       </c>
@@ -3344,15 +3345,15 @@
         <v>115</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="13.8" customHeight="1">
+    <row r="119" spans="1:6" ht="13.9" customHeight="1">
       <c r="A119" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B119" s="59"/>
-      <c r="C119" s="59"/>
-      <c r="D119" s="59"/>
-      <c r="E119" s="59"/>
-      <c r="F119" s="59"/>
+      <c r="B119" s="51"/>
+      <c r="C119" s="51"/>
+      <c r="D119" s="51"/>
+      <c r="E119" s="51"/>
+      <c r="F119" s="51"/>
     </row>
     <row r="120" spans="1:6">
       <c r="B120" s="10" t="s">
@@ -3382,6 +3383,24 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="B29:F29"/>
     <mergeCell ref="B111:F111"/>
     <mergeCell ref="B41:F41"/>
     <mergeCell ref="B115:F115"/>
@@ -3398,24 +3417,6 @@
     <mergeCell ref="B86:F86"/>
     <mergeCell ref="B62:F62"/>
     <mergeCell ref="B66:F66"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B37:F37"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -3423,44 +3424,44 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:J242"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E111" sqref="E111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.69921875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="9.19921875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="22.796875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.8984375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="31.59765625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32.59765625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.69921875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.19921875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.796875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.75" style="8" customWidth="1"/>
+    <col min="2" max="2" width="9.25" style="8" customWidth="1"/>
+    <col min="3" max="3" width="22.75" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.75" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.75" style="1" customWidth="1"/>
     <col min="10" max="10" width="35" style="8" customWidth="1"/>
-    <col min="11" max="16384" width="8.796875" style="8"/>
+    <col min="11" max="16384" width="8.75" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13.8" thickBot="1">
-      <c r="A1" s="77" t="s">
+    <row r="1" spans="1:10" ht="13.5" thickBot="1">
+      <c r="A1" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="79"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="81"/>
     </row>
     <row r="3" spans="1:10">
       <c r="B3" s="11" t="s">
@@ -3498,23 +3499,23 @@
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="1:10" ht="13.8" customHeight="1">
+    <row r="7" spans="1:10" ht="13.9" customHeight="1">
       <c r="A7" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="19">
         <v>1</v>
       </c>
-      <c r="C7" s="81" t="s">
+      <c r="C7" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="83"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="84"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="84"/>
+      <c r="H7" s="84"/>
+      <c r="I7" s="84"/>
+      <c r="J7" s="85"/>
     </row>
     <row r="8" spans="1:10" ht="30" customHeight="1">
       <c r="B8" s="20" t="s">
@@ -3545,7 +3546,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="29.4" customHeight="1">
+    <row r="9" spans="1:10" ht="29.45" customHeight="1">
       <c r="B9" s="23" t="s">
         <v>23</v>
       </c>
@@ -3564,9 +3565,9 @@
       <c r="G9" s="24"/>
       <c r="H9" s="17"/>
       <c r="I9" s="27"/>
-      <c r="J9" s="84"/>
-    </row>
-    <row r="10" spans="1:10" ht="13.8" customHeight="1">
+      <c r="J9" s="77"/>
+    </row>
+    <row r="10" spans="1:10" ht="13.9" customHeight="1">
       <c r="B10" s="25"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
@@ -3581,7 +3582,7 @@
       <c r="I10" s="17"/>
       <c r="J10" s="75"/>
     </row>
-    <row r="11" spans="1:10" ht="13.8" customHeight="1">
+    <row r="11" spans="1:10" ht="13.9" customHeight="1">
       <c r="B11" s="25"/>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
@@ -3596,7 +3597,7 @@
       <c r="I11" s="17"/>
       <c r="J11" s="75"/>
     </row>
-    <row r="12" spans="1:10" ht="13.8" customHeight="1">
+    <row r="12" spans="1:10" ht="13.9" customHeight="1">
       <c r="B12" s="25"/>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
@@ -3635,25 +3636,25 @@
       <c r="G14" s="24"/>
       <c r="H14" s="17"/>
       <c r="I14" s="17"/>
-      <c r="J14" s="85"/>
-    </row>
-    <row r="16" spans="1:10" ht="13.8" customHeight="1">
+      <c r="J14" s="78"/>
+    </row>
+    <row r="16" spans="1:10" ht="13.9" customHeight="1">
       <c r="A16" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B16" s="19">
         <v>2</v>
       </c>
-      <c r="C16" s="59" t="s">
+      <c r="C16" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="59"/>
-      <c r="E16" s="59"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="59"/>
-      <c r="H16" s="59"/>
-      <c r="I16" s="59"/>
-      <c r="J16" s="59"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="51"/>
     </row>
     <row r="17" spans="1:10" ht="30" customHeight="1">
       <c r="B17" s="20" t="s">
@@ -3703,9 +3704,9 @@
       <c r="G18" s="24"/>
       <c r="H18" s="17"/>
       <c r="I18" s="28"/>
-      <c r="J18" s="80"/>
-    </row>
-    <row r="19" spans="1:10" ht="13.8" customHeight="1">
+      <c r="J18" s="82"/>
+    </row>
+    <row r="19" spans="1:10" ht="13.9" customHeight="1">
       <c r="B19" s="25"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -3718,9 +3719,9 @@
       <c r="G19" s="24"/>
       <c r="H19" s="17"/>
       <c r="I19" s="28"/>
-      <c r="J19" s="80"/>
-    </row>
-    <row r="20" spans="1:10" ht="13.8" customHeight="1">
+      <c r="J19" s="82"/>
+    </row>
+    <row r="20" spans="1:10" ht="13.9" customHeight="1">
       <c r="B20" s="25"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
@@ -3731,9 +3732,9 @@
       <c r="G20" s="24"/>
       <c r="H20" s="17"/>
       <c r="I20" s="28"/>
-      <c r="J20" s="80"/>
-    </row>
-    <row r="21" spans="1:10" ht="13.8" customHeight="1">
+      <c r="J20" s="82"/>
+    </row>
+    <row r="21" spans="1:10" ht="13.9" customHeight="1">
       <c r="B21" s="25"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
@@ -3746,9 +3747,9 @@
       <c r="G21" s="24"/>
       <c r="H21" s="17"/>
       <c r="I21" s="28"/>
-      <c r="J21" s="80"/>
-    </row>
-    <row r="22" spans="1:10" ht="28.2" customHeight="1">
+      <c r="J21" s="82"/>
+    </row>
+    <row r="22" spans="1:10" ht="28.15" customHeight="1">
       <c r="B22" s="25"/>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
@@ -3761,9 +3762,9 @@
       <c r="G22" s="24"/>
       <c r="H22" s="17"/>
       <c r="I22" s="28"/>
-      <c r="J22" s="80"/>
-    </row>
-    <row r="23" spans="1:10" ht="16.8" customHeight="1">
+      <c r="J22" s="82"/>
+    </row>
+    <row r="23" spans="1:10" ht="16.899999999999999" customHeight="1">
       <c r="B23" s="25"/>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
@@ -3772,30 +3773,30 @@
       <c r="G23" s="24"/>
       <c r="H23" s="17"/>
       <c r="I23" s="28"/>
-      <c r="J23" s="80"/>
+      <c r="J23" s="82"/>
     </row>
     <row r="24" spans="1:10">
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="1:10" ht="13.8" customHeight="1">
+    <row r="25" spans="1:10" ht="13.9" customHeight="1">
       <c r="A25" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B25" s="19">
         <v>3</v>
       </c>
-      <c r="C25" s="59" t="s">
+      <c r="C25" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="59"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59"/>
-      <c r="G25" s="59"/>
-      <c r="H25" s="59"/>
-      <c r="I25" s="59"/>
-      <c r="J25" s="59"/>
-    </row>
-    <row r="26" spans="1:10" ht="13.8" customHeight="1">
+      <c r="D25" s="51"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="51"/>
+      <c r="H25" s="51"/>
+      <c r="I25" s="51"/>
+      <c r="J25" s="51"/>
+    </row>
+    <row r="26" spans="1:10" ht="13.9" customHeight="1">
       <c r="B26" s="20" t="s">
         <v>1</v>
       </c>
@@ -3845,7 +3846,7 @@
       <c r="I27" s="17"/>
       <c r="J27" s="74"/>
     </row>
-    <row r="28" spans="1:10" ht="13.8" customHeight="1">
+    <row r="28" spans="1:10" ht="13.9" customHeight="1">
       <c r="B28" s="25"/>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
@@ -3860,7 +3861,7 @@
       <c r="I28" s="17"/>
       <c r="J28" s="75"/>
     </row>
-    <row r="29" spans="1:10" ht="13.8" customHeight="1">
+    <row r="29" spans="1:10" ht="13.9" customHeight="1">
       <c r="B29" s="25"/>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
@@ -3875,7 +3876,7 @@
       <c r="I29" s="17"/>
       <c r="J29" s="75"/>
     </row>
-    <row r="30" spans="1:10" ht="13.8" customHeight="1">
+    <row r="30" spans="1:10" ht="13.9" customHeight="1">
       <c r="B30" s="25"/>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
@@ -3888,7 +3889,7 @@
       <c r="I30" s="17"/>
       <c r="J30" s="75"/>
     </row>
-    <row r="31" spans="1:10" ht="28.8" customHeight="1">
+    <row r="31" spans="1:10" ht="28.9" customHeight="1">
       <c r="B31" s="25"/>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
@@ -3914,25 +3915,25 @@
       <c r="I32" s="17"/>
       <c r="J32" s="76"/>
     </row>
-    <row r="34" spans="1:10" ht="13.8" customHeight="1">
+    <row r="34" spans="1:10" ht="13.9" customHeight="1">
       <c r="A34" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B34" s="19">
         <v>4</v>
       </c>
-      <c r="C34" s="59" t="s">
+      <c r="C34" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="59"/>
-      <c r="E34" s="59"/>
-      <c r="F34" s="59"/>
-      <c r="G34" s="59"/>
-      <c r="H34" s="59"/>
-      <c r="I34" s="59"/>
-      <c r="J34" s="59"/>
-    </row>
-    <row r="35" spans="1:10" ht="25.2" customHeight="1">
+      <c r="D34" s="51"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="51"/>
+      <c r="H34" s="51"/>
+      <c r="I34" s="51"/>
+      <c r="J34" s="51"/>
+    </row>
+    <row r="35" spans="1:10" ht="25.15" customHeight="1">
       <c r="B35" s="20" t="s">
         <v>1</v>
       </c>
@@ -3961,7 +3962,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="25.2" customHeight="1">
+    <row r="36" spans="1:10" ht="25.15" customHeight="1">
       <c r="B36" s="23" t="s">
         <v>26</v>
       </c>
@@ -3982,7 +3983,7 @@
       <c r="I36" s="17"/>
       <c r="J36" s="74"/>
     </row>
-    <row r="37" spans="1:10" ht="13.8" customHeight="1">
+    <row r="37" spans="1:10" ht="13.9" customHeight="1">
       <c r="B37" s="25"/>
       <c r="C37" s="17"/>
       <c r="D37" s="17"/>
@@ -3997,7 +3998,7 @@
       <c r="I37" s="17"/>
       <c r="J37" s="75"/>
     </row>
-    <row r="38" spans="1:10" ht="16.2" customHeight="1">
+    <row r="38" spans="1:10" ht="16.149999999999999" customHeight="1">
       <c r="B38" s="25"/>
       <c r="C38" s="17"/>
       <c r="D38" s="17"/>
@@ -4012,7 +4013,7 @@
       <c r="I38" s="17"/>
       <c r="J38" s="75"/>
     </row>
-    <row r="39" spans="1:10" ht="13.8" customHeight="1">
+    <row r="39" spans="1:10" ht="13.9" customHeight="1">
       <c r="B39" s="25"/>
       <c r="C39" s="17"/>
       <c r="D39" s="17"/>
@@ -4053,23 +4054,23 @@
       <c r="I41" s="17"/>
       <c r="J41" s="76"/>
     </row>
-    <row r="43" spans="1:10" ht="17.399999999999999" customHeight="1">
+    <row r="43" spans="1:10" ht="17.45" customHeight="1">
       <c r="A43" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B43" s="19">
         <v>5</v>
       </c>
-      <c r="C43" s="68" t="s">
+      <c r="C43" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="D43" s="69"/>
-      <c r="E43" s="69"/>
-      <c r="F43" s="69"/>
-      <c r="G43" s="69"/>
-      <c r="H43" s="69"/>
-      <c r="I43" s="69"/>
-      <c r="J43" s="70"/>
+      <c r="D43" s="61"/>
+      <c r="E43" s="61"/>
+      <c r="F43" s="61"/>
+      <c r="G43" s="61"/>
+      <c r="H43" s="61"/>
+      <c r="I43" s="61"/>
+      <c r="J43" s="62"/>
     </row>
     <row r="44" spans="1:10" ht="27" customHeight="1">
       <c r="B44" s="20" t="s">
@@ -4100,7 +4101,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="41.4" customHeight="1">
+    <row r="45" spans="1:10" ht="41.45" customHeight="1">
       <c r="B45" s="23" t="s">
         <v>28</v>
       </c>
@@ -4121,7 +4122,7 @@
       <c r="I45" s="17"/>
       <c r="J45" s="74"/>
     </row>
-    <row r="46" spans="1:10" ht="26.4" customHeight="1">
+    <row r="46" spans="1:10" ht="26.45" customHeight="1">
       <c r="B46" s="25"/>
       <c r="C46" s="17"/>
       <c r="D46" s="17"/>
@@ -4136,7 +4137,7 @@
       <c r="I46" s="17"/>
       <c r="J46" s="75"/>
     </row>
-    <row r="47" spans="1:10" ht="13.8" customHeight="1">
+    <row r="47" spans="1:10" ht="13.9" customHeight="1">
       <c r="B47" s="25"/>
       <c r="C47" s="17"/>
       <c r="D47" s="17"/>
@@ -4151,7 +4152,7 @@
       <c r="I47" s="17"/>
       <c r="J47" s="75"/>
     </row>
-    <row r="48" spans="1:10" ht="25.8" customHeight="1">
+    <row r="48" spans="1:10" ht="25.9" customHeight="1">
       <c r="B48" s="25"/>
       <c r="C48" s="17"/>
       <c r="D48" s="17"/>
@@ -4166,7 +4167,7 @@
       <c r="I48" s="17"/>
       <c r="J48" s="75"/>
     </row>
-    <row r="49" spans="1:10" ht="13.8" customHeight="1">
+    <row r="49" spans="1:10" ht="13.9" customHeight="1">
       <c r="B49" s="25"/>
       <c r="C49" s="17"/>
       <c r="D49" s="17"/>
@@ -4177,25 +4178,25 @@
       <c r="I49" s="17"/>
       <c r="J49" s="76"/>
     </row>
-    <row r="51" spans="1:10" ht="13.8" customHeight="1">
+    <row r="51" spans="1:10" ht="13.9" customHeight="1">
       <c r="A51" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B51" s="19">
         <v>6</v>
       </c>
-      <c r="C51" s="59" t="s">
+      <c r="C51" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="D51" s="59"/>
-      <c r="E51" s="59"/>
-      <c r="F51" s="59"/>
-      <c r="G51" s="59"/>
-      <c r="H51" s="59"/>
-      <c r="I51" s="59"/>
-      <c r="J51" s="59"/>
-    </row>
-    <row r="52" spans="1:10" ht="13.8" customHeight="1">
+      <c r="D51" s="51"/>
+      <c r="E51" s="51"/>
+      <c r="F51" s="51"/>
+      <c r="G51" s="51"/>
+      <c r="H51" s="51"/>
+      <c r="I51" s="51"/>
+      <c r="J51" s="51"/>
+    </row>
+    <row r="52" spans="1:10" ht="13.9" customHeight="1">
       <c r="B52" s="20" t="s">
         <v>1</v>
       </c>
@@ -4224,7 +4225,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="25.2" customHeight="1">
+    <row r="53" spans="1:10" ht="25.15" customHeight="1">
       <c r="B53" s="23" t="s">
         <v>30</v>
       </c>
@@ -4245,7 +4246,7 @@
       <c r="I53" s="17"/>
       <c r="J53" s="74"/>
     </row>
-    <row r="54" spans="1:10" ht="26.4" customHeight="1">
+    <row r="54" spans="1:10" ht="26.45" customHeight="1">
       <c r="B54" s="25"/>
       <c r="C54" s="17"/>
       <c r="D54" s="17"/>
@@ -4260,7 +4261,7 @@
       <c r="I54" s="17"/>
       <c r="J54" s="75"/>
     </row>
-    <row r="55" spans="1:10" ht="29.4" customHeight="1">
+    <row r="55" spans="1:10" ht="29.45" customHeight="1">
       <c r="B55" s="25"/>
       <c r="C55" s="17"/>
       <c r="D55" s="17"/>
@@ -4275,7 +4276,7 @@
       <c r="I55" s="17"/>
       <c r="J55" s="75"/>
     </row>
-    <row r="56" spans="1:10" ht="28.2" customHeight="1">
+    <row r="56" spans="1:10" ht="28.15" customHeight="1">
       <c r="B56" s="25"/>
       <c r="C56" s="17"/>
       <c r="D56" s="17"/>
@@ -4286,25 +4287,25 @@
       <c r="I56" s="17"/>
       <c r="J56" s="75"/>
     </row>
-    <row r="58" spans="1:10" ht="13.8" customHeight="1">
+    <row r="58" spans="1:10" ht="13.9" customHeight="1">
       <c r="A58" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B58" s="19">
         <v>7</v>
       </c>
-      <c r="C58" s="68" t="s">
+      <c r="C58" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="D58" s="69"/>
-      <c r="E58" s="69"/>
-      <c r="F58" s="69"/>
-      <c r="G58" s="69"/>
-      <c r="H58" s="69"/>
-      <c r="I58" s="69"/>
-      <c r="J58" s="70"/>
-    </row>
-    <row r="59" spans="1:10" ht="13.8" customHeight="1">
+      <c r="D58" s="61"/>
+      <c r="E58" s="61"/>
+      <c r="F58" s="61"/>
+      <c r="G58" s="61"/>
+      <c r="H58" s="61"/>
+      <c r="I58" s="61"/>
+      <c r="J58" s="62"/>
+    </row>
+    <row r="59" spans="1:10" ht="13.9" customHeight="1">
       <c r="B59" s="20" t="s">
         <v>1</v>
       </c>
@@ -4333,7 +4334,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="40.200000000000003" customHeight="1">
+    <row r="60" spans="1:10" ht="40.15" customHeight="1">
       <c r="B60" s="23" t="s">
         <v>39</v>
       </c>
@@ -4354,7 +4355,7 @@
       <c r="I60" s="17"/>
       <c r="J60" s="74"/>
     </row>
-    <row r="61" spans="1:10" ht="13.8" customHeight="1">
+    <row r="61" spans="1:10" ht="13.9" customHeight="1">
       <c r="B61" s="25"/>
       <c r="C61" s="17"/>
       <c r="D61" s="17"/>
@@ -4369,7 +4370,7 @@
       <c r="I61" s="17"/>
       <c r="J61" s="75"/>
     </row>
-    <row r="62" spans="1:10" ht="28.8" customHeight="1">
+    <row r="62" spans="1:10" ht="28.9" customHeight="1">
       <c r="B62" s="25"/>
       <c r="C62" s="17"/>
       <c r="D62" s="17"/>
@@ -4384,7 +4385,7 @@
       <c r="I62" s="17"/>
       <c r="J62" s="75"/>
     </row>
-    <row r="63" spans="1:10" ht="13.8" customHeight="1">
+    <row r="63" spans="1:10" ht="13.9" customHeight="1">
       <c r="B63" s="25"/>
       <c r="C63" s="17"/>
       <c r="D63" s="17"/>
@@ -4414,7 +4415,7 @@
       <c r="I64" s="17"/>
       <c r="J64" s="75"/>
     </row>
-    <row r="65" spans="1:10" ht="17.399999999999999" customHeight="1">
+    <row r="65" spans="1:10" ht="17.45" customHeight="1">
       <c r="B65" s="25"/>
       <c r="C65" s="17"/>
       <c r="D65" s="17"/>
@@ -4425,25 +4426,25 @@
       <c r="I65" s="17"/>
       <c r="J65" s="76"/>
     </row>
-    <row r="67" spans="1:10" ht="13.8" customHeight="1">
+    <row r="67" spans="1:10" ht="13.9" customHeight="1">
       <c r="A67" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B67" s="19">
         <v>8</v>
       </c>
-      <c r="C67" s="59" t="s">
+      <c r="C67" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="D67" s="59"/>
-      <c r="E67" s="59"/>
-      <c r="F67" s="59"/>
-      <c r="G67" s="59"/>
-      <c r="H67" s="59"/>
-      <c r="I67" s="59"/>
-      <c r="J67" s="59"/>
-    </row>
-    <row r="68" spans="1:10" ht="13.8" customHeight="1">
+      <c r="D67" s="51"/>
+      <c r="E67" s="51"/>
+      <c r="F67" s="51"/>
+      <c r="G67" s="51"/>
+      <c r="H67" s="51"/>
+      <c r="I67" s="51"/>
+      <c r="J67" s="51"/>
+    </row>
+    <row r="68" spans="1:10" ht="13.9" customHeight="1">
       <c r="B68" s="20" t="s">
         <v>1</v>
       </c>
@@ -4493,7 +4494,7 @@
       <c r="I69" s="17"/>
       <c r="J69" s="74"/>
     </row>
-    <row r="70" spans="1:10" ht="13.8" customHeight="1">
+    <row r="70" spans="1:10" ht="13.9" customHeight="1">
       <c r="B70" s="25"/>
       <c r="C70" s="17"/>
       <c r="D70" s="17"/>
@@ -4508,7 +4509,7 @@
       <c r="I70" s="17"/>
       <c r="J70" s="75"/>
     </row>
-    <row r="71" spans="1:10" ht="16.8" customHeight="1">
+    <row r="71" spans="1:10" ht="16.899999999999999" customHeight="1">
       <c r="B71" s="25"/>
       <c r="C71" s="17"/>
       <c r="D71" s="17"/>
@@ -4538,7 +4539,7 @@
       <c r="I72" s="17"/>
       <c r="J72" s="75"/>
     </row>
-    <row r="73" spans="1:10" ht="38.4" customHeight="1">
+    <row r="73" spans="1:10" ht="38.450000000000003" customHeight="1">
       <c r="B73" s="25"/>
       <c r="C73" s="17"/>
       <c r="D73" s="17"/>
@@ -4564,25 +4565,25 @@
       <c r="I74" s="17"/>
       <c r="J74" s="76"/>
     </row>
-    <row r="76" spans="1:10" ht="13.8" customHeight="1">
+    <row r="76" spans="1:10" ht="13.9" customHeight="1">
       <c r="A76" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B76" s="19">
         <v>9</v>
       </c>
-      <c r="C76" s="59" t="s">
+      <c r="C76" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="D76" s="59"/>
-      <c r="E76" s="59"/>
-      <c r="F76" s="59"/>
-      <c r="G76" s="59"/>
-      <c r="H76" s="59"/>
-      <c r="I76" s="59"/>
-      <c r="J76" s="59"/>
-    </row>
-    <row r="77" spans="1:10" ht="13.8" customHeight="1">
+      <c r="D76" s="51"/>
+      <c r="E76" s="51"/>
+      <c r="F76" s="51"/>
+      <c r="G76" s="51"/>
+      <c r="H76" s="51"/>
+      <c r="I76" s="51"/>
+      <c r="J76" s="51"/>
+    </row>
+    <row r="77" spans="1:10" ht="13.9" customHeight="1">
       <c r="B77" s="20" t="s">
         <v>1</v>
       </c>
@@ -4611,7 +4612,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="25.2" customHeight="1">
+    <row r="78" spans="1:10" ht="25.15" customHeight="1">
       <c r="B78" s="23" t="s">
         <v>35</v>
       </c>
@@ -4632,7 +4633,7 @@
       <c r="I78" s="17"/>
       <c r="J78" s="74"/>
     </row>
-    <row r="79" spans="1:10" ht="13.8" customHeight="1">
+    <row r="79" spans="1:10" ht="13.9" customHeight="1">
       <c r="B79" s="25"/>
       <c r="C79" s="17"/>
       <c r="D79" s="17"/>
@@ -4647,7 +4648,7 @@
       <c r="I79" s="17"/>
       <c r="J79" s="75"/>
     </row>
-    <row r="80" spans="1:10" ht="13.8" customHeight="1">
+    <row r="80" spans="1:10" ht="13.9" customHeight="1">
       <c r="B80" s="25"/>
       <c r="C80" s="17"/>
       <c r="D80" s="17"/>
@@ -4709,25 +4710,25 @@
       <c r="I84" s="47"/>
       <c r="J84" s="48"/>
     </row>
-    <row r="86" spans="1:10" ht="13.8" customHeight="1">
+    <row r="86" spans="1:10" ht="13.9" customHeight="1">
       <c r="A86" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B86" s="19">
         <v>1</v>
       </c>
-      <c r="C86" s="59" t="s">
+      <c r="C86" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="D86" s="59"/>
-      <c r="E86" s="59"/>
-      <c r="F86" s="59"/>
-      <c r="G86" s="59"/>
-      <c r="H86" s="59"/>
-      <c r="I86" s="59"/>
-      <c r="J86" s="59"/>
-    </row>
-    <row r="87" spans="1:10" ht="13.8" customHeight="1">
+      <c r="D86" s="51"/>
+      <c r="E86" s="51"/>
+      <c r="F86" s="51"/>
+      <c r="G86" s="51"/>
+      <c r="H86" s="51"/>
+      <c r="I86" s="51"/>
+      <c r="J86" s="51"/>
+    </row>
+    <row r="87" spans="1:10" ht="13.9" customHeight="1">
       <c r="B87" s="20" t="s">
         <v>1</v>
       </c>
@@ -4777,7 +4778,7 @@
       <c r="I88" s="17"/>
       <c r="J88" s="74"/>
     </row>
-    <row r="89" spans="1:10" ht="29.4" customHeight="1">
+    <row r="89" spans="1:10" ht="29.45" customHeight="1">
       <c r="B89" s="25"/>
       <c r="C89" s="17"/>
       <c r="D89" s="17"/>
@@ -4792,7 +4793,7 @@
       <c r="I89" s="17"/>
       <c r="J89" s="75"/>
     </row>
-    <row r="90" spans="1:10" ht="13.8" customHeight="1">
+    <row r="90" spans="1:10" ht="13.9" customHeight="1">
       <c r="B90" s="25"/>
       <c r="C90" s="17"/>
       <c r="D90" s="17"/>
@@ -4807,7 +4808,7 @@
       <c r="I90" s="17"/>
       <c r="J90" s="75"/>
     </row>
-    <row r="91" spans="1:10" ht="13.8" customHeight="1">
+    <row r="91" spans="1:10" ht="13.9" customHeight="1">
       <c r="B91" s="25"/>
       <c r="C91" s="17"/>
       <c r="D91" s="17"/>
@@ -4822,7 +4823,7 @@
       <c r="I91" s="17"/>
       <c r="J91" s="75"/>
     </row>
-    <row r="92" spans="1:10" ht="53.4" customHeight="1">
+    <row r="92" spans="1:10" ht="53.45" customHeight="1">
       <c r="B92" s="25"/>
       <c r="C92" s="17"/>
       <c r="D92" s="17"/>
@@ -4848,25 +4849,25 @@
       <c r="I93" s="17"/>
       <c r="J93" s="76"/>
     </row>
-    <row r="95" spans="1:10" ht="13.8" customHeight="1">
+    <row r="95" spans="1:10" ht="13.9" customHeight="1">
       <c r="A95" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B95" s="19">
         <v>2</v>
       </c>
-      <c r="C95" s="59" t="s">
+      <c r="C95" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="D95" s="59"/>
-      <c r="E95" s="59"/>
-      <c r="F95" s="59"/>
-      <c r="G95" s="59"/>
-      <c r="H95" s="59"/>
-      <c r="I95" s="59"/>
-      <c r="J95" s="59"/>
-    </row>
-    <row r="96" spans="1:10" ht="13.8" customHeight="1">
+      <c r="D95" s="51"/>
+      <c r="E95" s="51"/>
+      <c r="F95" s="51"/>
+      <c r="G95" s="51"/>
+      <c r="H95" s="51"/>
+      <c r="I95" s="51"/>
+      <c r="J95" s="51"/>
+    </row>
+    <row r="96" spans="1:10" ht="13.9" customHeight="1">
       <c r="B96" s="20" t="s">
         <v>1</v>
       </c>
@@ -4895,7 +4896,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="40.799999999999997" customHeight="1">
+    <row r="97" spans="1:10" ht="40.9" customHeight="1">
       <c r="B97" s="23" t="s">
         <v>35</v>
       </c>
@@ -4916,7 +4917,7 @@
       <c r="I97" s="17"/>
       <c r="J97" s="74"/>
     </row>
-    <row r="98" spans="1:10" ht="13.8" customHeight="1">
+    <row r="98" spans="1:10" ht="13.9" customHeight="1">
       <c r="B98" s="25"/>
       <c r="C98" s="17"/>
       <c r="D98" s="17"/>
@@ -4929,7 +4930,7 @@
       <c r="I98" s="17"/>
       <c r="J98" s="75"/>
     </row>
-    <row r="99" spans="1:10" ht="13.8" customHeight="1">
+    <row r="99" spans="1:10" ht="13.9" customHeight="1">
       <c r="B99" s="25"/>
       <c r="C99" s="17"/>
       <c r="D99" s="17"/>
@@ -4944,7 +4945,7 @@
       <c r="I99" s="17"/>
       <c r="J99" s="75"/>
     </row>
-    <row r="100" spans="1:10" ht="20.399999999999999" customHeight="1">
+    <row r="100" spans="1:10" ht="20.45" customHeight="1">
       <c r="B100" s="25"/>
       <c r="C100" s="17"/>
       <c r="D100" s="17"/>
@@ -4959,7 +4960,7 @@
       <c r="I100" s="17"/>
       <c r="J100" s="75"/>
     </row>
-    <row r="101" spans="1:10" ht="40.200000000000003" customHeight="1">
+    <row r="101" spans="1:10" ht="40.15" customHeight="1">
       <c r="B101" s="25"/>
       <c r="C101" s="17"/>
       <c r="D101" s="17"/>
@@ -4985,25 +4986,25 @@
       <c r="I102" s="17"/>
       <c r="J102" s="76"/>
     </row>
-    <row r="104" spans="1:10" ht="13.8" customHeight="1">
+    <row r="104" spans="1:10" ht="13.9" customHeight="1">
       <c r="A104" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B104" s="19">
         <v>3</v>
       </c>
-      <c r="C104" s="59" t="s">
+      <c r="C104" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="D104" s="59"/>
-      <c r="E104" s="59"/>
-      <c r="F104" s="59"/>
-      <c r="G104" s="59"/>
-      <c r="H104" s="59"/>
-      <c r="I104" s="59"/>
-      <c r="J104" s="59"/>
-    </row>
-    <row r="105" spans="1:10" ht="13.8" customHeight="1">
+      <c r="D104" s="51"/>
+      <c r="E104" s="51"/>
+      <c r="F104" s="51"/>
+      <c r="G104" s="51"/>
+      <c r="H104" s="51"/>
+      <c r="I104" s="51"/>
+      <c r="J104" s="51"/>
+    </row>
+    <row r="105" spans="1:10" ht="13.9" customHeight="1">
       <c r="B105" s="20" t="s">
         <v>1</v>
       </c>
@@ -5032,7 +5033,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="40.799999999999997" customHeight="1">
+    <row r="106" spans="1:10" ht="40.9" customHeight="1">
       <c r="B106" s="23" t="s">
         <v>36</v>
       </c>
@@ -5068,7 +5069,7 @@
       <c r="I107" s="17"/>
       <c r="J107" s="75"/>
     </row>
-    <row r="108" spans="1:10" ht="13.8" customHeight="1">
+    <row r="108" spans="1:10" ht="13.9" customHeight="1">
       <c r="B108" s="25"/>
       <c r="C108" s="17"/>
       <c r="D108" s="17"/>
@@ -5083,7 +5084,7 @@
       <c r="I108" s="17"/>
       <c r="J108" s="75"/>
     </row>
-    <row r="109" spans="1:10" ht="13.8" customHeight="1">
+    <row r="109" spans="1:10" ht="13.9" customHeight="1">
       <c r="B109" s="25"/>
       <c r="C109" s="17"/>
       <c r="D109" s="17"/>
@@ -5098,7 +5099,7 @@
       <c r="I109" s="17"/>
       <c r="J109" s="75"/>
     </row>
-    <row r="110" spans="1:10" ht="43.2" customHeight="1">
+    <row r="110" spans="1:10" ht="43.15" customHeight="1">
       <c r="B110" s="25"/>
       <c r="C110" s="17"/>
       <c r="D110" s="17"/>
@@ -5124,25 +5125,25 @@
       <c r="I111" s="17"/>
       <c r="J111" s="76"/>
     </row>
-    <row r="113" spans="1:10" ht="13.8" customHeight="1">
+    <row r="113" spans="1:10" ht="13.9" customHeight="1">
       <c r="A113" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B113" s="19">
         <v>4</v>
       </c>
-      <c r="C113" s="59" t="s">
+      <c r="C113" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="D113" s="59"/>
-      <c r="E113" s="59"/>
-      <c r="F113" s="59"/>
-      <c r="G113" s="59"/>
-      <c r="H113" s="59"/>
-      <c r="I113" s="59"/>
-      <c r="J113" s="59"/>
-    </row>
-    <row r="114" spans="1:10" ht="13.8" customHeight="1">
+      <c r="D113" s="51"/>
+      <c r="E113" s="51"/>
+      <c r="F113" s="51"/>
+      <c r="G113" s="51"/>
+      <c r="H113" s="51"/>
+      <c r="I113" s="51"/>
+      <c r="J113" s="51"/>
+    </row>
+    <row r="114" spans="1:10" ht="13.9" customHeight="1">
       <c r="B114" s="20" t="s">
         <v>1</v>
       </c>
@@ -5171,7 +5172,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="40.799999999999997" customHeight="1">
+    <row r="115" spans="1:10" ht="40.9" customHeight="1">
       <c r="B115" s="23" t="s">
         <v>37</v>
       </c>
@@ -5207,7 +5208,7 @@
       <c r="I116" s="17"/>
       <c r="J116" s="75"/>
     </row>
-    <row r="117" spans="1:10" ht="13.8" customHeight="1">
+    <row r="117" spans="1:10" ht="13.9" customHeight="1">
       <c r="B117" s="25"/>
       <c r="C117" s="17"/>
       <c r="D117" s="17"/>
@@ -5222,7 +5223,7 @@
       <c r="I117" s="17"/>
       <c r="J117" s="75"/>
     </row>
-    <row r="118" spans="1:10" ht="13.8" customHeight="1">
+    <row r="118" spans="1:10" ht="13.9" customHeight="1">
       <c r="B118" s="25"/>
       <c r="C118" s="17"/>
       <c r="D118" s="17"/>
@@ -5237,7 +5238,7 @@
       <c r="I118" s="17"/>
       <c r="J118" s="75"/>
     </row>
-    <row r="119" spans="1:10" ht="40.200000000000003" customHeight="1">
+    <row r="119" spans="1:10" ht="40.15" customHeight="1">
       <c r="B119" s="25"/>
       <c r="C119" s="17"/>
       <c r="D119" s="17"/>
@@ -5263,25 +5264,25 @@
       <c r="I120" s="17"/>
       <c r="J120" s="76"/>
     </row>
-    <row r="122" spans="1:10" ht="13.8" customHeight="1">
+    <row r="122" spans="1:10" ht="13.9" customHeight="1">
       <c r="A122" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B122" s="19">
         <v>5</v>
       </c>
-      <c r="C122" s="59" t="s">
+      <c r="C122" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="D122" s="59"/>
-      <c r="E122" s="59"/>
-      <c r="F122" s="59"/>
-      <c r="G122" s="59"/>
-      <c r="H122" s="59"/>
-      <c r="I122" s="59"/>
-      <c r="J122" s="59"/>
-    </row>
-    <row r="123" spans="1:10" ht="13.8" customHeight="1">
+      <c r="D122" s="51"/>
+      <c r="E122" s="51"/>
+      <c r="F122" s="51"/>
+      <c r="G122" s="51"/>
+      <c r="H122" s="51"/>
+      <c r="I122" s="51"/>
+      <c r="J122" s="51"/>
+    </row>
+    <row r="123" spans="1:10" ht="13.9" customHeight="1">
       <c r="B123" s="20" t="s">
         <v>1</v>
       </c>
@@ -5310,7 +5311,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="124" spans="1:10" ht="40.799999999999997" customHeight="1">
+    <row r="124" spans="1:10" ht="40.9" customHeight="1">
       <c r="B124" s="23" t="s">
         <v>53</v>
       </c>
@@ -5331,7 +5332,7 @@
       <c r="I124" s="17"/>
       <c r="J124" s="74"/>
     </row>
-    <row r="125" spans="1:10" ht="17.399999999999999" customHeight="1">
+    <row r="125" spans="1:10" ht="17.45" customHeight="1">
       <c r="B125" s="25"/>
       <c r="C125" s="17"/>
       <c r="D125" s="17"/>
@@ -5346,7 +5347,7 @@
       <c r="I125" s="17"/>
       <c r="J125" s="75"/>
     </row>
-    <row r="126" spans="1:10" ht="13.8" customHeight="1">
+    <row r="126" spans="1:10" ht="13.9" customHeight="1">
       <c r="B126" s="25"/>
       <c r="C126" s="17"/>
       <c r="D126" s="17"/>
@@ -5361,7 +5362,7 @@
       <c r="I126" s="17"/>
       <c r="J126" s="75"/>
     </row>
-    <row r="127" spans="1:10" ht="13.8" customHeight="1">
+    <row r="127" spans="1:10" ht="13.9" customHeight="1">
       <c r="B127" s="25"/>
       <c r="C127" s="17"/>
       <c r="D127" s="17"/>
@@ -5374,7 +5375,7 @@
       <c r="I127" s="17"/>
       <c r="J127" s="75"/>
     </row>
-    <row r="128" spans="1:10" ht="40.799999999999997" customHeight="1">
+    <row r="128" spans="1:10" ht="40.9" customHeight="1">
       <c r="B128" s="25"/>
       <c r="C128" s="17"/>
       <c r="D128" s="17"/>
@@ -5400,25 +5401,25 @@
       <c r="I129" s="17"/>
       <c r="J129" s="76"/>
     </row>
-    <row r="131" spans="1:10" ht="13.8" customHeight="1">
+    <row r="131" spans="1:10" ht="13.9" customHeight="1">
       <c r="A131" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B131" s="19">
         <v>6</v>
       </c>
-      <c r="C131" s="59" t="s">
+      <c r="C131" s="51" t="s">
         <v>136</v>
       </c>
-      <c r="D131" s="59"/>
-      <c r="E131" s="59"/>
-      <c r="F131" s="59"/>
-      <c r="G131" s="59"/>
-      <c r="H131" s="59"/>
-      <c r="I131" s="59"/>
-      <c r="J131" s="59"/>
-    </row>
-    <row r="132" spans="1:10" ht="13.8" customHeight="1">
+      <c r="D131" s="51"/>
+      <c r="E131" s="51"/>
+      <c r="F131" s="51"/>
+      <c r="G131" s="51"/>
+      <c r="H131" s="51"/>
+      <c r="I131" s="51"/>
+      <c r="J131" s="51"/>
+    </row>
+    <row r="132" spans="1:10" ht="13.9" customHeight="1">
       <c r="B132" s="20" t="s">
         <v>1</v>
       </c>
@@ -5447,7 +5448,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="133" spans="1:10" ht="52.8">
+    <row r="133" spans="1:10" ht="51">
       <c r="B133" s="23" t="s">
         <v>56</v>
       </c>
@@ -5468,7 +5469,7 @@
       <c r="I133" s="17"/>
       <c r="J133" s="74"/>
     </row>
-    <row r="134" spans="1:10" ht="13.8" customHeight="1">
+    <row r="134" spans="1:10" ht="13.9" customHeight="1">
       <c r="B134" s="25"/>
       <c r="C134" s="17"/>
       <c r="D134" s="17"/>
@@ -5483,7 +5484,7 @@
       <c r="I134" s="17"/>
       <c r="J134" s="75"/>
     </row>
-    <row r="135" spans="1:10" ht="13.8" customHeight="1">
+    <row r="135" spans="1:10" ht="13.9" customHeight="1">
       <c r="B135" s="25"/>
       <c r="C135" s="17"/>
       <c r="D135" s="17"/>
@@ -5513,7 +5514,7 @@
       <c r="I136" s="17"/>
       <c r="J136" s="75"/>
     </row>
-    <row r="137" spans="1:10" ht="40.200000000000003" customHeight="1">
+    <row r="137" spans="1:10" ht="40.15" customHeight="1">
       <c r="B137" s="25"/>
       <c r="C137" s="17"/>
       <c r="D137" s="17"/>
@@ -5539,25 +5540,25 @@
       <c r="I138" s="17"/>
       <c r="J138" s="76"/>
     </row>
-    <row r="140" spans="1:10" ht="13.8" customHeight="1">
+    <row r="140" spans="1:10" ht="13.9" customHeight="1">
       <c r="A140" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B140" s="19">
         <v>7</v>
       </c>
-      <c r="C140" s="59" t="s">
+      <c r="C140" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="D140" s="59"/>
-      <c r="E140" s="59"/>
-      <c r="F140" s="59"/>
-      <c r="G140" s="59"/>
-      <c r="H140" s="59"/>
-      <c r="I140" s="59"/>
-      <c r="J140" s="59"/>
-    </row>
-    <row r="141" spans="1:10" ht="13.8" customHeight="1">
+      <c r="D140" s="51"/>
+      <c r="E140" s="51"/>
+      <c r="F140" s="51"/>
+      <c r="G140" s="51"/>
+      <c r="H140" s="51"/>
+      <c r="I140" s="51"/>
+      <c r="J140" s="51"/>
+    </row>
+    <row r="141" spans="1:10" ht="13.9" customHeight="1">
       <c r="B141" s="20" t="s">
         <v>1</v>
       </c>
@@ -5586,7 +5587,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="142" spans="1:10" ht="40.799999999999997" customHeight="1">
+    <row r="142" spans="1:10" ht="40.9" customHeight="1">
       <c r="B142" s="23" t="s">
         <v>62</v>
       </c>
@@ -5607,7 +5608,7 @@
       <c r="I142" s="17"/>
       <c r="J142" s="74"/>
     </row>
-    <row r="143" spans="1:10" ht="13.8" customHeight="1">
+    <row r="143" spans="1:10" ht="13.9" customHeight="1">
       <c r="B143" s="25"/>
       <c r="C143" s="17"/>
       <c r="D143" s="17"/>
@@ -5622,7 +5623,7 @@
       <c r="I143" s="17"/>
       <c r="J143" s="75"/>
     </row>
-    <row r="144" spans="1:10" ht="13.8" customHeight="1">
+    <row r="144" spans="1:10" ht="13.9" customHeight="1">
       <c r="B144" s="25"/>
       <c r="C144" s="17"/>
       <c r="D144" s="17"/>
@@ -5650,7 +5651,7 @@
       <c r="I145" s="17"/>
       <c r="J145" s="75"/>
     </row>
-    <row r="146" spans="1:10" ht="34.799999999999997" customHeight="1">
+    <row r="146" spans="1:10" ht="34.9" customHeight="1">
       <c r="B146" s="25"/>
       <c r="C146" s="17"/>
       <c r="D146" s="17"/>
@@ -5676,25 +5677,25 @@
       <c r="I147" s="17"/>
       <c r="J147" s="76"/>
     </row>
-    <row r="149" spans="1:10" ht="13.8" customHeight="1">
+    <row r="149" spans="1:10" ht="13.9" customHeight="1">
       <c r="A149" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B149" s="19">
         <v>8</v>
       </c>
-      <c r="C149" s="59" t="s">
+      <c r="C149" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="D149" s="59"/>
-      <c r="E149" s="59"/>
-      <c r="F149" s="59"/>
-      <c r="G149" s="59"/>
-      <c r="H149" s="59"/>
-      <c r="I149" s="59"/>
-      <c r="J149" s="59"/>
-    </row>
-    <row r="150" spans="1:10" ht="13.8" customHeight="1">
+      <c r="D149" s="51"/>
+      <c r="E149" s="51"/>
+      <c r="F149" s="51"/>
+      <c r="G149" s="51"/>
+      <c r="H149" s="51"/>
+      <c r="I149" s="51"/>
+      <c r="J149" s="51"/>
+    </row>
+    <row r="150" spans="1:10" ht="13.9" customHeight="1">
       <c r="B150" s="20" t="s">
         <v>1</v>
       </c>
@@ -5723,7 +5724,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="151" spans="1:10" ht="40.799999999999997" customHeight="1">
+    <row r="151" spans="1:10" ht="40.9" customHeight="1">
       <c r="B151" s="23" t="s">
         <v>64</v>
       </c>
@@ -5744,7 +5745,7 @@
       <c r="I151" s="17"/>
       <c r="J151" s="74"/>
     </row>
-    <row r="152" spans="1:10" ht="13.8" customHeight="1">
+    <row r="152" spans="1:10" ht="13.9" customHeight="1">
       <c r="B152" s="25"/>
       <c r="C152" s="17"/>
       <c r="D152" s="17"/>
@@ -5759,7 +5760,7 @@
       <c r="I152" s="17"/>
       <c r="J152" s="75"/>
     </row>
-    <row r="153" spans="1:10" ht="29.4" customHeight="1">
+    <row r="153" spans="1:10" ht="29.45" customHeight="1">
       <c r="B153" s="25"/>
       <c r="C153" s="17"/>
       <c r="D153" s="17"/>
@@ -5774,7 +5775,7 @@
       <c r="I153" s="17"/>
       <c r="J153" s="75"/>
     </row>
-    <row r="154" spans="1:10" ht="13.8" customHeight="1">
+    <row r="154" spans="1:10" ht="13.9" customHeight="1">
       <c r="B154" s="25"/>
       <c r="C154" s="17"/>
       <c r="D154" s="17"/>
@@ -5815,25 +5816,25 @@
       <c r="I156" s="17"/>
       <c r="J156" s="76"/>
     </row>
-    <row r="158" spans="1:10" ht="13.8" customHeight="1">
+    <row r="158" spans="1:10" ht="13.9" customHeight="1">
       <c r="A158" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B158" s="19">
         <v>9</v>
       </c>
-      <c r="C158" s="59" t="s">
+      <c r="C158" s="51" t="s">
         <v>141</v>
       </c>
-      <c r="D158" s="59"/>
-      <c r="E158" s="59"/>
-      <c r="F158" s="59"/>
-      <c r="G158" s="59"/>
-      <c r="H158" s="59"/>
-      <c r="I158" s="59"/>
-      <c r="J158" s="59"/>
-    </row>
-    <row r="159" spans="1:10" ht="13.8" customHeight="1">
+      <c r="D158" s="51"/>
+      <c r="E158" s="51"/>
+      <c r="F158" s="51"/>
+      <c r="G158" s="51"/>
+      <c r="H158" s="51"/>
+      <c r="I158" s="51"/>
+      <c r="J158" s="51"/>
+    </row>
+    <row r="159" spans="1:10" ht="13.9" customHeight="1">
       <c r="B159" s="20" t="s">
         <v>1</v>
       </c>
@@ -5862,7 +5863,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="160" spans="1:10" ht="40.799999999999997" customHeight="1">
+    <row r="160" spans="1:10" ht="40.9" customHeight="1">
       <c r="B160" s="23" t="s">
         <v>67</v>
       </c>
@@ -5883,7 +5884,7 @@
       <c r="I160" s="17"/>
       <c r="J160" s="74"/>
     </row>
-    <row r="161" spans="1:10" ht="13.8" customHeight="1">
+    <row r="161" spans="1:10" ht="13.9" customHeight="1">
       <c r="B161" s="25"/>
       <c r="C161" s="17"/>
       <c r="D161" s="17"/>
@@ -5913,7 +5914,7 @@
       <c r="I162" s="17"/>
       <c r="J162" s="75"/>
     </row>
-    <row r="163" spans="1:10" ht="13.8" customHeight="1">
+    <row r="163" spans="1:10" ht="13.9" customHeight="1">
       <c r="B163" s="25"/>
       <c r="C163" s="17"/>
       <c r="D163" s="17"/>
@@ -5954,25 +5955,25 @@
       <c r="I165" s="17"/>
       <c r="J165" s="76"/>
     </row>
-    <row r="167" spans="1:10" ht="13.8" customHeight="1">
+    <row r="167" spans="1:10" ht="13.9" customHeight="1">
       <c r="A167" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B167" s="19">
         <v>10</v>
       </c>
-      <c r="C167" s="59" t="s">
+      <c r="C167" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="D167" s="59"/>
-      <c r="E167" s="59"/>
-      <c r="F167" s="59"/>
-      <c r="G167" s="59"/>
-      <c r="H167" s="59"/>
-      <c r="I167" s="59"/>
-      <c r="J167" s="59"/>
-    </row>
-    <row r="168" spans="1:10" ht="13.8" customHeight="1">
+      <c r="D167" s="51"/>
+      <c r="E167" s="51"/>
+      <c r="F167" s="51"/>
+      <c r="G167" s="51"/>
+      <c r="H167" s="51"/>
+      <c r="I167" s="51"/>
+      <c r="J167" s="51"/>
+    </row>
+    <row r="168" spans="1:10" ht="13.9" customHeight="1">
       <c r="B168" s="20" t="s">
         <v>1</v>
       </c>
@@ -6001,7 +6002,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="169" spans="1:10" ht="40.799999999999997" customHeight="1">
+    <row r="169" spans="1:10" ht="40.9" customHeight="1">
       <c r="B169" s="23" t="s">
         <v>68</v>
       </c>
@@ -6022,7 +6023,7 @@
       <c r="I169" s="17"/>
       <c r="J169" s="74"/>
     </row>
-    <row r="170" spans="1:10" ht="26.4" customHeight="1">
+    <row r="170" spans="1:10" ht="26.45" customHeight="1">
       <c r="B170" s="25"/>
       <c r="C170" s="17"/>
       <c r="D170" s="17"/>
@@ -6048,25 +6049,25 @@
       <c r="I171" s="17"/>
       <c r="J171" s="76"/>
     </row>
-    <row r="173" spans="1:10" ht="13.8" customHeight="1">
+    <row r="173" spans="1:10" ht="13.9" customHeight="1">
       <c r="A173" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B173" s="19">
         <v>11</v>
       </c>
-      <c r="C173" s="59" t="s">
+      <c r="C173" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="D173" s="59"/>
-      <c r="E173" s="59"/>
-      <c r="F173" s="59"/>
-      <c r="G173" s="59"/>
-      <c r="H173" s="59"/>
-      <c r="I173" s="59"/>
-      <c r="J173" s="59"/>
-    </row>
-    <row r="174" spans="1:10" ht="13.8" customHeight="1">
+      <c r="D173" s="51"/>
+      <c r="E173" s="51"/>
+      <c r="F173" s="51"/>
+      <c r="G173" s="51"/>
+      <c r="H173" s="51"/>
+      <c r="I173" s="51"/>
+      <c r="J173" s="51"/>
+    </row>
+    <row r="174" spans="1:10" ht="13.9" customHeight="1">
       <c r="B174" s="20" t="s">
         <v>1</v>
       </c>
@@ -6095,7 +6096,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="175" spans="1:10" ht="40.799999999999997" customHeight="1">
+    <row r="175" spans="1:10" ht="40.9" customHeight="1">
       <c r="B175" s="23" t="s">
         <v>71</v>
       </c>
@@ -6131,7 +6132,7 @@
       <c r="I176" s="17"/>
       <c r="J176" s="75"/>
     </row>
-    <row r="177" spans="1:10" ht="13.8" customHeight="1">
+    <row r="177" spans="1:10" ht="13.9" customHeight="1">
       <c r="B177" s="25"/>
       <c r="C177" s="17"/>
       <c r="D177" s="17"/>
@@ -6146,7 +6147,7 @@
       <c r="I177" s="17"/>
       <c r="J177" s="75"/>
     </row>
-    <row r="178" spans="1:10" ht="13.8" customHeight="1">
+    <row r="178" spans="1:10" ht="13.9" customHeight="1">
       <c r="B178" s="25"/>
       <c r="C178" s="17"/>
       <c r="D178" s="17"/>
@@ -6161,7 +6162,7 @@
       <c r="I178" s="17"/>
       <c r="J178" s="75"/>
     </row>
-    <row r="179" spans="1:10" ht="19.8" customHeight="1">
+    <row r="179" spans="1:10" ht="19.899999999999999" customHeight="1">
       <c r="B179" s="25"/>
       <c r="C179" s="17"/>
       <c r="D179" s="17"/>
@@ -6191,25 +6192,25 @@
       <c r="I180" s="17"/>
       <c r="J180" s="76"/>
     </row>
-    <row r="182" spans="1:10" ht="13.8" customHeight="1">
+    <row r="182" spans="1:10" ht="13.9" customHeight="1">
       <c r="A182" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B182" s="19">
         <v>12</v>
       </c>
-      <c r="C182" s="59" t="s">
+      <c r="C182" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="D182" s="59"/>
-      <c r="E182" s="59"/>
-      <c r="F182" s="59"/>
-      <c r="G182" s="59"/>
-      <c r="H182" s="59"/>
-      <c r="I182" s="59"/>
-      <c r="J182" s="59"/>
-    </row>
-    <row r="183" spans="1:10" ht="13.8" customHeight="1">
+      <c r="D182" s="51"/>
+      <c r="E182" s="51"/>
+      <c r="F182" s="51"/>
+      <c r="G182" s="51"/>
+      <c r="H182" s="51"/>
+      <c r="I182" s="51"/>
+      <c r="J182" s="51"/>
+    </row>
+    <row r="183" spans="1:10" ht="13.9" customHeight="1">
       <c r="B183" s="20" t="s">
         <v>1</v>
       </c>
@@ -6238,7 +6239,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:10" ht="40.799999999999997" customHeight="1">
+    <row r="184" spans="1:10" ht="40.9" customHeight="1">
       <c r="B184" s="23" t="s">
         <v>72</v>
       </c>
@@ -6259,7 +6260,7 @@
       <c r="I184" s="17"/>
       <c r="J184" s="74"/>
     </row>
-    <row r="185" spans="1:10" ht="13.8" customHeight="1">
+    <row r="185" spans="1:10" ht="13.9" customHeight="1">
       <c r="B185" s="25"/>
       <c r="C185" s="17"/>
       <c r="D185" s="17"/>
@@ -6274,7 +6275,7 @@
       <c r="I185" s="17"/>
       <c r="J185" s="75"/>
     </row>
-    <row r="186" spans="1:10" ht="13.8" customHeight="1">
+    <row r="186" spans="1:10" ht="13.9" customHeight="1">
       <c r="B186" s="25"/>
       <c r="C186" s="17"/>
       <c r="D186" s="17"/>
@@ -6289,7 +6290,7 @@
       <c r="I186" s="17"/>
       <c r="J186" s="75"/>
     </row>
-    <row r="187" spans="1:10" ht="13.8" customHeight="1">
+    <row r="187" spans="1:10" ht="13.9" customHeight="1">
       <c r="B187" s="25"/>
       <c r="C187" s="17"/>
       <c r="D187" s="17"/>
@@ -6304,7 +6305,7 @@
       <c r="I187" s="17"/>
       <c r="J187" s="75"/>
     </row>
-    <row r="188" spans="1:10" ht="37.799999999999997" customHeight="1">
+    <row r="188" spans="1:10" ht="37.9" customHeight="1">
       <c r="B188" s="25"/>
       <c r="C188" s="17"/>
       <c r="D188" s="17"/>
@@ -6336,7 +6337,7 @@
       <c r="I189" s="17"/>
       <c r="J189" s="75"/>
     </row>
-    <row r="190" spans="1:10" ht="25.8" customHeight="1">
+    <row r="190" spans="1:10" ht="25.9" customHeight="1">
       <c r="B190" s="25"/>
       <c r="C190" s="17"/>
       <c r="D190" s="17"/>
@@ -6351,7 +6352,7 @@
       <c r="I190" s="17"/>
       <c r="J190" s="75"/>
     </row>
-    <row r="191" spans="1:10" ht="31.2" customHeight="1">
+    <row r="191" spans="1:10" ht="31.15" customHeight="1">
       <c r="B191" s="25"/>
       <c r="C191" s="17"/>
       <c r="D191" s="17"/>
@@ -6366,7 +6367,7 @@
       <c r="I191" s="17"/>
       <c r="J191" s="75"/>
     </row>
-    <row r="192" spans="1:10" ht="29.4" customHeight="1">
+    <row r="192" spans="1:10" ht="29.45" customHeight="1">
       <c r="B192" s="25"/>
       <c r="C192" s="17"/>
       <c r="D192" s="17"/>
@@ -6407,25 +6408,25 @@
       <c r="I194" s="17"/>
       <c r="J194" s="76"/>
     </row>
-    <row r="196" spans="1:10" ht="13.8" customHeight="1">
+    <row r="196" spans="1:10" ht="13.9" customHeight="1">
       <c r="A196" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B196" s="19">
         <v>13</v>
       </c>
-      <c r="C196" s="59" t="s">
+      <c r="C196" s="51" t="s">
         <v>93</v>
       </c>
-      <c r="D196" s="59"/>
-      <c r="E196" s="59"/>
-      <c r="F196" s="59"/>
-      <c r="G196" s="59"/>
-      <c r="H196" s="59"/>
-      <c r="I196" s="59"/>
-      <c r="J196" s="59"/>
-    </row>
-    <row r="197" spans="1:10" ht="13.8" customHeight="1">
+      <c r="D196" s="51"/>
+      <c r="E196" s="51"/>
+      <c r="F196" s="51"/>
+      <c r="G196" s="51"/>
+      <c r="H196" s="51"/>
+      <c r="I196" s="51"/>
+      <c r="J196" s="51"/>
+    </row>
+    <row r="197" spans="1:10" ht="13.9" customHeight="1">
       <c r="B197" s="20" t="s">
         <v>1</v>
       </c>
@@ -6454,7 +6455,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="198" spans="1:10" ht="40.799999999999997" customHeight="1">
+    <row r="198" spans="1:10" ht="40.9" customHeight="1">
       <c r="B198" s="23" t="s">
         <v>75</v>
       </c>
@@ -6475,7 +6476,7 @@
       <c r="I198" s="17"/>
       <c r="J198" s="74"/>
     </row>
-    <row r="199" spans="1:10" ht="13.8" customHeight="1">
+    <row r="199" spans="1:10" ht="13.9" customHeight="1">
       <c r="B199" s="25"/>
       <c r="C199" s="17"/>
       <c r="D199" s="17"/>
@@ -6488,7 +6489,7 @@
       <c r="I199" s="17"/>
       <c r="J199" s="75"/>
     </row>
-    <row r="200" spans="1:10" ht="13.8" customHeight="1">
+    <row r="200" spans="1:10" ht="13.9" customHeight="1">
       <c r="B200" s="25"/>
       <c r="C200" s="17"/>
       <c r="D200" s="17"/>
@@ -6501,7 +6502,7 @@
       <c r="I200" s="17"/>
       <c r="J200" s="75"/>
     </row>
-    <row r="201" spans="1:10" ht="13.8" customHeight="1">
+    <row r="201" spans="1:10" ht="13.9" customHeight="1">
       <c r="B201" s="25"/>
       <c r="C201" s="17"/>
       <c r="D201" s="17"/>
@@ -6540,25 +6541,25 @@
       <c r="I203" s="17"/>
       <c r="J203" s="76"/>
     </row>
-    <row r="205" spans="1:10" ht="13.8" customHeight="1">
+    <row r="205" spans="1:10" ht="13.9" customHeight="1">
       <c r="A205" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B205" s="19">
         <v>14</v>
       </c>
-      <c r="C205" s="59" t="s">
+      <c r="C205" s="51" t="s">
         <v>99</v>
       </c>
-      <c r="D205" s="59"/>
-      <c r="E205" s="59"/>
-      <c r="F205" s="59"/>
-      <c r="G205" s="59"/>
-      <c r="H205" s="59"/>
-      <c r="I205" s="59"/>
-      <c r="J205" s="59"/>
-    </row>
-    <row r="206" spans="1:10" ht="13.8" customHeight="1">
+      <c r="D205" s="51"/>
+      <c r="E205" s="51"/>
+      <c r="F205" s="51"/>
+      <c r="G205" s="51"/>
+      <c r="H205" s="51"/>
+      <c r="I205" s="51"/>
+      <c r="J205" s="51"/>
+    </row>
+    <row r="206" spans="1:10" ht="13.9" customHeight="1">
       <c r="B206" s="20" t="s">
         <v>1</v>
       </c>
@@ -6587,7 +6588,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="207" spans="1:10" ht="40.799999999999997" customHeight="1">
+    <row r="207" spans="1:10" ht="40.9" customHeight="1">
       <c r="B207" s="23" t="s">
         <v>77</v>
       </c>
@@ -6608,7 +6609,7 @@
       <c r="I207" s="17"/>
       <c r="J207" s="74"/>
     </row>
-    <row r="208" spans="1:10" ht="13.8" customHeight="1">
+    <row r="208" spans="1:10" ht="13.9" customHeight="1">
       <c r="B208" s="25"/>
       <c r="C208" s="17"/>
       <c r="D208" s="17"/>
@@ -6623,7 +6624,7 @@
       <c r="I208" s="17"/>
       <c r="J208" s="75"/>
     </row>
-    <row r="209" spans="1:10" ht="13.8" customHeight="1">
+    <row r="209" spans="1:10" ht="13.9" customHeight="1">
       <c r="B209" s="25"/>
       <c r="C209" s="17"/>
       <c r="D209" s="17"/>
@@ -6638,7 +6639,7 @@
       <c r="I209" s="17"/>
       <c r="J209" s="75"/>
     </row>
-    <row r="210" spans="1:10" ht="13.8" customHeight="1">
+    <row r="210" spans="1:10" ht="13.9" customHeight="1">
       <c r="B210" s="25"/>
       <c r="C210" s="17"/>
       <c r="D210" s="17"/>
@@ -6653,7 +6654,7 @@
       <c r="I210" s="17"/>
       <c r="J210" s="75"/>
     </row>
-    <row r="211" spans="1:10" ht="28.2" customHeight="1">
+    <row r="211" spans="1:10" ht="28.15" customHeight="1">
       <c r="B211" s="25"/>
       <c r="C211" s="17"/>
       <c r="D211" s="17"/>
@@ -6668,7 +6669,7 @@
       <c r="I211" s="17"/>
       <c r="J211" s="75"/>
     </row>
-    <row r="212" spans="1:10" ht="28.8" customHeight="1">
+    <row r="212" spans="1:10" ht="28.9" customHeight="1">
       <c r="B212" s="25"/>
       <c r="C212" s="17"/>
       <c r="D212" s="17"/>
@@ -6683,7 +6684,7 @@
       <c r="I212" s="17"/>
       <c r="J212" s="75"/>
     </row>
-    <row r="213" spans="1:10" ht="14.4" customHeight="1">
+    <row r="213" spans="1:10" ht="14.45" customHeight="1">
       <c r="B213" s="25"/>
       <c r="C213" s="17"/>
       <c r="D213" s="17"/>
@@ -6694,25 +6695,25 @@
       <c r="I213" s="17"/>
       <c r="J213" s="76"/>
     </row>
-    <row r="215" spans="1:10" ht="13.8" customHeight="1">
+    <row r="215" spans="1:10" ht="13.9" customHeight="1">
       <c r="A215" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B215" s="19">
         <v>15</v>
       </c>
-      <c r="C215" s="59" t="s">
+      <c r="C215" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="D215" s="59"/>
-      <c r="E215" s="59"/>
-      <c r="F215" s="59"/>
-      <c r="G215" s="59"/>
-      <c r="H215" s="59"/>
-      <c r="I215" s="59"/>
-      <c r="J215" s="59"/>
-    </row>
-    <row r="216" spans="1:10" ht="13.8" customHeight="1">
+      <c r="D215" s="51"/>
+      <c r="E215" s="51"/>
+      <c r="F215" s="51"/>
+      <c r="G215" s="51"/>
+      <c r="H215" s="51"/>
+      <c r="I215" s="51"/>
+      <c r="J215" s="51"/>
+    </row>
+    <row r="216" spans="1:10" ht="13.9" customHeight="1">
       <c r="B216" s="20" t="s">
         <v>1</v>
       </c>
@@ -6741,7 +6742,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="217" spans="1:10" ht="40.799999999999997" customHeight="1">
+    <row r="217" spans="1:10" ht="40.9" customHeight="1">
       <c r="B217" s="23" t="s">
         <v>78</v>
       </c>
@@ -6762,7 +6763,7 @@
       <c r="I217" s="17"/>
       <c r="J217" s="74"/>
     </row>
-    <row r="218" spans="1:10" ht="13.8" customHeight="1">
+    <row r="218" spans="1:10" ht="13.9" customHeight="1">
       <c r="B218" s="25"/>
       <c r="C218" s="17"/>
       <c r="D218" s="17"/>
@@ -6777,7 +6778,7 @@
       <c r="I218" s="17"/>
       <c r="J218" s="75"/>
     </row>
-    <row r="219" spans="1:10" ht="13.8" customHeight="1">
+    <row r="219" spans="1:10" ht="13.9" customHeight="1">
       <c r="B219" s="25"/>
       <c r="C219" s="17"/>
       <c r="D219" s="17"/>
@@ -6792,7 +6793,7 @@
       <c r="I219" s="17"/>
       <c r="J219" s="75"/>
     </row>
-    <row r="220" spans="1:10" ht="13.8" customHeight="1">
+    <row r="220" spans="1:10" ht="13.9" customHeight="1">
       <c r="B220" s="25"/>
       <c r="C220" s="17"/>
       <c r="D220" s="17"/>
@@ -6837,25 +6838,25 @@
       <c r="I222" s="17"/>
       <c r="J222" s="76"/>
     </row>
-    <row r="224" spans="1:10" ht="13.8" customHeight="1">
+    <row r="224" spans="1:10" ht="13.9" customHeight="1">
       <c r="A224" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B224" s="19">
         <v>16</v>
       </c>
-      <c r="C224" s="59" t="s">
+      <c r="C224" s="51" t="s">
         <v>104</v>
       </c>
-      <c r="D224" s="59"/>
-      <c r="E224" s="59"/>
-      <c r="F224" s="59"/>
-      <c r="G224" s="59"/>
-      <c r="H224" s="59"/>
-      <c r="I224" s="59"/>
-      <c r="J224" s="59"/>
-    </row>
-    <row r="225" spans="1:10" ht="13.8" customHeight="1">
+      <c r="D224" s="51"/>
+      <c r="E224" s="51"/>
+      <c r="F224" s="51"/>
+      <c r="G224" s="51"/>
+      <c r="H224" s="51"/>
+      <c r="I224" s="51"/>
+      <c r="J224" s="51"/>
+    </row>
+    <row r="225" spans="1:10" ht="13.9" customHeight="1">
       <c r="B225" s="20" t="s">
         <v>1</v>
       </c>
@@ -6884,7 +6885,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="226" spans="1:10" ht="40.799999999999997" customHeight="1">
+    <row r="226" spans="1:10" ht="40.9" customHeight="1">
       <c r="B226" s="23" t="s">
         <v>86</v>
       </c>
@@ -6905,7 +6906,7 @@
       <c r="I226" s="17"/>
       <c r="J226" s="74"/>
     </row>
-    <row r="227" spans="1:10" ht="13.8" customHeight="1">
+    <row r="227" spans="1:10" ht="13.9" customHeight="1">
       <c r="B227" s="25"/>
       <c r="C227" s="17"/>
       <c r="D227" s="17"/>
@@ -6920,7 +6921,7 @@
       <c r="I227" s="17"/>
       <c r="J227" s="75"/>
     </row>
-    <row r="228" spans="1:10" ht="13.8" customHeight="1">
+    <row r="228" spans="1:10" ht="13.9" customHeight="1">
       <c r="B228" s="25"/>
       <c r="C228" s="17"/>
       <c r="D228" s="17"/>
@@ -6935,7 +6936,7 @@
       <c r="I228" s="17"/>
       <c r="J228" s="75"/>
     </row>
-    <row r="229" spans="1:10" ht="13.8" customHeight="1">
+    <row r="229" spans="1:10" ht="13.9" customHeight="1">
       <c r="B229" s="25"/>
       <c r="C229" s="17"/>
       <c r="D229" s="17"/>
@@ -6980,25 +6981,25 @@
       <c r="I231" s="17"/>
       <c r="J231" s="76"/>
     </row>
-    <row r="233" spans="1:10" ht="13.8" customHeight="1">
+    <row r="233" spans="1:10" ht="13.9" customHeight="1">
       <c r="A233" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B233" s="19">
         <v>17</v>
       </c>
-      <c r="C233" s="59" t="s">
+      <c r="C233" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="D233" s="59"/>
-      <c r="E233" s="59"/>
-      <c r="F233" s="59"/>
-      <c r="G233" s="59"/>
-      <c r="H233" s="59"/>
-      <c r="I233" s="59"/>
-      <c r="J233" s="59"/>
-    </row>
-    <row r="234" spans="1:10" ht="13.8" customHeight="1">
+      <c r="D233" s="51"/>
+      <c r="E233" s="51"/>
+      <c r="F233" s="51"/>
+      <c r="G233" s="51"/>
+      <c r="H233" s="51"/>
+      <c r="I233" s="51"/>
+      <c r="J233" s="51"/>
+    </row>
+    <row r="234" spans="1:10" ht="13.9" customHeight="1">
       <c r="B234" s="20" t="s">
         <v>1</v>
       </c>
@@ -7027,7 +7028,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="235" spans="1:10" ht="40.799999999999997" customHeight="1">
+    <row r="235" spans="1:10" ht="40.9" customHeight="1">
       <c r="B235" s="23" t="s">
         <v>92</v>
       </c>
@@ -7074,25 +7075,25 @@
       <c r="I237" s="17"/>
       <c r="J237" s="76"/>
     </row>
-    <row r="239" spans="1:10" ht="13.8" customHeight="1">
+    <row r="239" spans="1:10" ht="13.9" customHeight="1">
       <c r="A239" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B239" s="19">
         <v>18</v>
       </c>
-      <c r="C239" s="59" t="s">
+      <c r="C239" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="D239" s="59"/>
-      <c r="E239" s="59"/>
-      <c r="F239" s="59"/>
-      <c r="G239" s="59"/>
-      <c r="H239" s="59"/>
-      <c r="I239" s="59"/>
-      <c r="J239" s="59"/>
-    </row>
-    <row r="240" spans="1:10" ht="13.8" customHeight="1">
+      <c r="D239" s="51"/>
+      <c r="E239" s="51"/>
+      <c r="F239" s="51"/>
+      <c r="G239" s="51"/>
+      <c r="H239" s="51"/>
+      <c r="I239" s="51"/>
+      <c r="J239" s="51"/>
+    </row>
+    <row r="240" spans="1:10" ht="13.9" customHeight="1">
       <c r="B240" s="20" t="s">
         <v>1</v>
       </c>
@@ -7121,7 +7122,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="241" spans="2:10" ht="40.799999999999997" customHeight="1">
+    <row r="241" spans="2:10" ht="40.9" customHeight="1">
       <c r="B241" s="23" t="s">
         <v>107</v>
       </c>
@@ -7155,13 +7156,38 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="J88:J93"/>
-    <mergeCell ref="J97:J102"/>
-    <mergeCell ref="C43:J43"/>
-    <mergeCell ref="J9:J14"/>
-    <mergeCell ref="J60:J65"/>
-    <mergeCell ref="J69:J74"/>
-    <mergeCell ref="J78:J82"/>
+    <mergeCell ref="C239:J239"/>
+    <mergeCell ref="J241:J242"/>
+    <mergeCell ref="J217:J222"/>
+    <mergeCell ref="C224:J224"/>
+    <mergeCell ref="J226:J231"/>
+    <mergeCell ref="C233:J233"/>
+    <mergeCell ref="J235:J237"/>
+    <mergeCell ref="C196:J196"/>
+    <mergeCell ref="J198:J203"/>
+    <mergeCell ref="C205:J205"/>
+    <mergeCell ref="J207:J213"/>
+    <mergeCell ref="C215:J215"/>
+    <mergeCell ref="J169:J171"/>
+    <mergeCell ref="C173:J173"/>
+    <mergeCell ref="J175:J180"/>
+    <mergeCell ref="C182:J182"/>
+    <mergeCell ref="J184:J194"/>
+    <mergeCell ref="C149:J149"/>
+    <mergeCell ref="J151:J156"/>
+    <mergeCell ref="C158:J158"/>
+    <mergeCell ref="J160:J165"/>
+    <mergeCell ref="C167:J167"/>
+    <mergeCell ref="J124:J129"/>
+    <mergeCell ref="C131:J131"/>
+    <mergeCell ref="J133:J138"/>
+    <mergeCell ref="C140:J140"/>
+    <mergeCell ref="J142:J147"/>
+    <mergeCell ref="C104:J104"/>
+    <mergeCell ref="J106:J111"/>
+    <mergeCell ref="C113:J113"/>
+    <mergeCell ref="J115:J120"/>
+    <mergeCell ref="C122:J122"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="J27:J32"/>
     <mergeCell ref="C86:J86"/>
@@ -7178,40 +7204,15 @@
     <mergeCell ref="C16:J16"/>
     <mergeCell ref="C25:J25"/>
     <mergeCell ref="C34:J34"/>
-    <mergeCell ref="C104:J104"/>
-    <mergeCell ref="J106:J111"/>
-    <mergeCell ref="C113:J113"/>
-    <mergeCell ref="J115:J120"/>
-    <mergeCell ref="C122:J122"/>
-    <mergeCell ref="J124:J129"/>
-    <mergeCell ref="C131:J131"/>
-    <mergeCell ref="J133:J138"/>
-    <mergeCell ref="C140:J140"/>
-    <mergeCell ref="J142:J147"/>
-    <mergeCell ref="C149:J149"/>
-    <mergeCell ref="J151:J156"/>
-    <mergeCell ref="C158:J158"/>
-    <mergeCell ref="J160:J165"/>
-    <mergeCell ref="C167:J167"/>
-    <mergeCell ref="J169:J171"/>
-    <mergeCell ref="C173:J173"/>
-    <mergeCell ref="J175:J180"/>
-    <mergeCell ref="C182:J182"/>
-    <mergeCell ref="J184:J194"/>
-    <mergeCell ref="C196:J196"/>
-    <mergeCell ref="J198:J203"/>
-    <mergeCell ref="C205:J205"/>
-    <mergeCell ref="J207:J213"/>
-    <mergeCell ref="C215:J215"/>
-    <mergeCell ref="C239:J239"/>
-    <mergeCell ref="J241:J242"/>
-    <mergeCell ref="J217:J222"/>
-    <mergeCell ref="C224:J224"/>
-    <mergeCell ref="J226:J231"/>
-    <mergeCell ref="C233:J233"/>
-    <mergeCell ref="J235:J237"/>
+    <mergeCell ref="J88:J93"/>
+    <mergeCell ref="J97:J102"/>
+    <mergeCell ref="C43:J43"/>
+    <mergeCell ref="J9:J14"/>
+    <mergeCell ref="J60:J65"/>
+    <mergeCell ref="J69:J74"/>
+    <mergeCell ref="J78:J82"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
criando test case account e income
</commit_message>
<xml_diff>
--- a/app_moneytracker/relatorios/Relatory - Test Case Specification and Report.xlsx
+++ b/app_moneytracker/relatorios/Relatory - Test Case Specification and Report.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="516" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="516" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Requisitos" sheetId="5" r:id="rId1"/>
@@ -749,7 +749,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -1300,16 +1300,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1332,6 +1326,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1920,14 +1920,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
@@ -1937,9 +1937,9 @@
       <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <sheetData>
-    <row r="25" spans="2:6" ht="15">
+    <row r="25" spans="2:6">
       <c r="B25" s="34"/>
       <c r="C25" s="50"/>
       <c r="D25" s="50"/>
@@ -1957,25 +1957,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:F121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="10.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.25" style="2" customWidth="1"/>
-    <col min="4" max="4" width="25.75" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.3984375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.8984375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.19921875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="25.69921875" style="2" customWidth="1"/>
     <col min="5" max="5" width="41" style="2" customWidth="1"/>
-    <col min="6" max="6" width="29.125" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.75" style="8"/>
+    <col min="6" max="6" width="29.09765625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.69921875" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.6" customHeight="1" thickBot="1">
@@ -2008,7 +2008,7 @@
       <c r="B4" s="70"/>
       <c r="C4" s="71"/>
     </row>
-    <row r="5" spans="1:6" ht="17.45" customHeight="1">
+    <row r="5" spans="1:6" ht="17.399999999999999" customHeight="1">
       <c r="A5" s="36" t="s">
         <v>0</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.9" customHeight="1">
+    <row r="9" spans="1:6" ht="13.95" customHeight="1">
       <c r="A9" s="9" t="s">
         <v>0</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="38.25">
+    <row r="11" spans="1:6" ht="39.6">
       <c r="B11" s="6" t="s">
         <v>24</v>
       </c>
@@ -2104,7 +2104,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" ht="13.9" customHeight="1">
+    <row r="13" spans="1:6" ht="13.95" customHeight="1">
       <c r="A13" s="9" t="s">
         <v>0</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="51">
+    <row r="15" spans="1:6" ht="52.8">
       <c r="B15" s="6" t="s">
         <v>25</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.9" customHeight="1">
+    <row r="17" spans="1:6" ht="13.95" customHeight="1">
       <c r="A17" s="9" t="s">
         <v>0</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="38.25">
+    <row r="19" spans="1:6" ht="39.6">
       <c r="B19" s="6" t="s">
         <v>26</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="22.15" customHeight="1">
+    <row r="21" spans="1:6" ht="22.2" customHeight="1">
       <c r="A21" s="9" t="s">
         <v>0</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="38.25">
+    <row r="23" spans="1:6" ht="52.8">
       <c r="B23" s="4" t="s">
         <v>28</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="13.9" customHeight="1">
+    <row r="25" spans="1:6" ht="13.95" customHeight="1">
       <c r="A25" s="9" t="s">
         <v>0</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="38.25">
+    <row r="27" spans="1:6" ht="39.6">
       <c r="B27" s="4" t="s">
         <v>30</v>
       </c>
@@ -2295,7 +2295,7 @@
       <c r="E28" s="38"/>
       <c r="F28" s="38"/>
     </row>
-    <row r="29" spans="1:6" ht="13.9" customHeight="1">
+    <row r="29" spans="1:6" ht="13.95" customHeight="1">
       <c r="A29" s="9" t="s">
         <v>0</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="38.25">
+    <row r="31" spans="1:6" ht="39.6">
       <c r="B31" s="4" t="s">
         <v>39</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="38.25">
+    <row r="35" spans="1:6" ht="39.6">
       <c r="B35" s="4" t="s">
         <v>49</v>
       </c>
@@ -2430,7 +2430,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="40.9" customHeight="1">
+    <row r="39" spans="1:6" ht="40.950000000000003" customHeight="1">
       <c r="B39" s="4" t="s">
         <v>52</v>
       </c>
@@ -2490,21 +2490,21 @@
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
     </row>
-    <row r="44" spans="1:6" ht="13.5" thickBot="1">
+    <row r="44" spans="1:6" ht="13.8" thickBot="1">
       <c r="B44" s="37"/>
       <c r="C44" s="37"/>
       <c r="D44" s="37"/>
       <c r="E44" s="38"/>
       <c r="F44" s="38"/>
     </row>
-    <row r="45" spans="1:6" ht="13.9" customHeight="1" thickBot="1">
+    <row r="45" spans="1:6" ht="13.95" customHeight="1" thickBot="1">
       <c r="A45" s="69" t="s">
         <v>32</v>
       </c>
       <c r="B45" s="72"/>
       <c r="C45" s="73"/>
     </row>
-    <row r="46" spans="1:6" ht="16.149999999999999" customHeight="1">
+    <row r="46" spans="1:6" ht="16.2" customHeight="1">
       <c r="A46" s="9" t="s">
         <v>0</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="63.75">
+    <row r="48" spans="1:6" ht="66">
       <c r="B48" s="4" t="s">
         <v>34</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="13.9" customHeight="1">
+    <row r="50" spans="1:6" ht="13.95" customHeight="1">
       <c r="A50" s="9" t="s">
         <v>0</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="38.25">
+    <row r="52" spans="1:6" ht="39.6">
       <c r="B52" s="4" t="s">
         <v>35</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="13.9" customHeight="1">
+    <row r="54" spans="1:6" ht="13.95" customHeight="1">
       <c r="A54" s="9" t="s">
         <v>0</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="38.25">
+    <row r="56" spans="1:6" ht="39.6">
       <c r="B56" s="4" t="s">
         <v>36</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="13.9" customHeight="1">
+    <row r="58" spans="1:6" ht="13.95" customHeight="1">
       <c r="A58" s="9" t="s">
         <v>0</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="63.75">
+    <row r="60" spans="1:6" ht="66">
       <c r="B60" s="4" t="s">
         <v>37</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="13.9" customHeight="1">
+    <row r="62" spans="1:6" ht="13.95" customHeight="1">
       <c r="A62" s="9" t="s">
         <v>0</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="38.25">
+    <row r="64" spans="1:6" ht="39.6">
       <c r="B64" s="4" t="s">
         <v>53</v>
       </c>
@@ -2734,7 +2734,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="13.9" customHeight="1">
+    <row r="66" spans="1:6" ht="13.95" customHeight="1">
       <c r="A66" s="9" t="s">
         <v>0</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="51">
+    <row r="68" spans="1:6" ht="52.8">
       <c r="B68" s="4" t="s">
         <v>56</v>
       </c>
@@ -2780,7 +2780,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="13.9" customHeight="1">
+    <row r="70" spans="1:6" ht="13.95" customHeight="1">
       <c r="A70" s="9" t="s">
         <v>0</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="38.25">
+    <row r="72" spans="1:6" ht="39.6">
       <c r="B72" s="4" t="s">
         <v>62</v>
       </c>
@@ -2826,7 +2826,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="13.9" customHeight="1">
+    <row r="74" spans="1:6" ht="13.95" customHeight="1">
       <c r="A74" s="9" t="s">
         <v>0</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="38.25">
+    <row r="76" spans="1:6" ht="39.6">
       <c r="B76" s="4" t="s">
         <v>64</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="13.9" customHeight="1">
+    <row r="78" spans="1:6" ht="13.95" customHeight="1">
       <c r="A78" s="9" t="s">
         <v>0</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="51">
+    <row r="80" spans="1:6" ht="52.8">
       <c r="B80" s="4" t="s">
         <v>67</v>
       </c>
@@ -2918,7 +2918,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="13.9" customHeight="1">
+    <row r="82" spans="1:6" ht="13.95" customHeight="1">
       <c r="A82" s="9" t="s">
         <v>0</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="38.25">
+    <row r="84" spans="1:6" ht="39.6">
       <c r="B84" s="4" t="s">
         <v>68</v>
       </c>
@@ -2964,7 +2964,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="13.9" customHeight="1">
+    <row r="86" spans="1:6" ht="13.95" customHeight="1">
       <c r="A86" s="9" t="s">
         <v>0</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="38.25">
+    <row r="88" spans="1:6" ht="39.6">
       <c r="B88" s="4" t="s">
         <v>71</v>
       </c>
@@ -3010,7 +3010,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="13.9" customHeight="1">
+    <row r="90" spans="1:6" ht="13.95" customHeight="1">
       <c r="A90" s="9" t="s">
         <v>0</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="38.25">
+    <row r="92" spans="1:6" ht="39.6">
       <c r="B92" s="4" t="s">
         <v>72</v>
       </c>
@@ -3056,7 +3056,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="41.45" customHeight="1">
+    <row r="93" spans="1:6" ht="41.4" customHeight="1">
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
       <c r="D93" s="4" t="s">
@@ -3069,7 +3069,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="13.9" customHeight="1">
+    <row r="95" spans="1:6" ht="13.95" customHeight="1">
       <c r="A95" s="9" t="s">
         <v>0</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="38.25">
+    <row r="97" spans="1:6" ht="39.6">
       <c r="B97" s="4" t="s">
         <v>75</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="13.9" customHeight="1">
+    <row r="99" spans="1:6" ht="13.95" customHeight="1">
       <c r="A99" s="9" t="s">
         <v>0</v>
       </c>
@@ -3144,7 +3144,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="51">
+    <row r="101" spans="1:6" ht="52.8">
       <c r="B101" s="4" t="s">
         <v>77</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="13.9" customHeight="1">
+    <row r="103" spans="1:6" ht="13.95" customHeight="1">
       <c r="A103" s="9" t="s">
         <v>0</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="63.75">
+    <row r="105" spans="1:6" ht="66">
       <c r="B105" s="4" t="s">
         <v>78</v>
       </c>
@@ -3207,7 +3207,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="13.9" customHeight="1">
+    <row r="107" spans="1:6" ht="13.95" customHeight="1">
       <c r="A107" s="9" t="s">
         <v>0</v>
       </c>
@@ -3236,7 +3236,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="63.75">
+    <row r="109" spans="1:6" ht="66">
       <c r="B109" s="4" t="s">
         <v>86</v>
       </c>
@@ -3253,7 +3253,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="13.9" customHeight="1">
+    <row r="111" spans="1:6" ht="13.95" customHeight="1">
       <c r="A111" s="9" t="s">
         <v>0</v>
       </c>
@@ -3282,7 +3282,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="25.5">
+    <row r="113" spans="1:6" ht="26.4">
       <c r="B113" s="4" t="s">
         <v>92</v>
       </c>
@@ -3299,7 +3299,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="13.9" customHeight="1">
+    <row r="115" spans="1:6" ht="13.95" customHeight="1">
       <c r="A115" s="9" t="s">
         <v>0</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="38.25">
+    <row r="117" spans="1:6" ht="39.6">
       <c r="B117" s="4" t="s">
         <v>107</v>
       </c>
@@ -3345,7 +3345,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="13.9" customHeight="1">
+    <row r="119" spans="1:6" ht="13.95" customHeight="1">
       <c r="A119" s="9" t="s">
         <v>0</v>
       </c>
@@ -3383,24 +3383,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="B29:F29"/>
     <mergeCell ref="B111:F111"/>
     <mergeCell ref="B41:F41"/>
     <mergeCell ref="B115:F115"/>
@@ -3417,51 +3399,69 @@
     <mergeCell ref="B86:F86"/>
     <mergeCell ref="B62:F62"/>
     <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="A4:C4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:J242"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E111" sqref="E111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="14.75" style="8" customWidth="1"/>
-    <col min="2" max="2" width="9.25" style="8" customWidth="1"/>
-    <col min="3" max="3" width="22.75" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="31.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32.625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.75" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.25" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.75" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.69921875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="9.19921875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="22.69921875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.8984375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31.59765625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.59765625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.69921875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.19921875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.69921875" style="1" customWidth="1"/>
     <col min="10" max="10" width="35" style="8" customWidth="1"/>
-    <col min="11" max="16384" width="8.75" style="8"/>
+    <col min="11" max="16384" width="8.69921875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13.5" thickBot="1">
-      <c r="A1" s="79" t="s">
+    <row r="1" spans="1:10" ht="13.8" thickBot="1">
+      <c r="A1" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="81"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="79"/>
     </row>
     <row r="3" spans="1:10">
       <c r="B3" s="11" t="s">
@@ -3499,23 +3499,23 @@
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="1:10" ht="13.9" customHeight="1">
+    <row r="7" spans="1:10" ht="13.95" customHeight="1">
       <c r="A7" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="19">
         <v>1</v>
       </c>
-      <c r="C7" s="83" t="s">
+      <c r="C7" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="84"/>
-      <c r="I7" s="84"/>
-      <c r="J7" s="85"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="83"/>
     </row>
     <row r="8" spans="1:10" ht="30" customHeight="1">
       <c r="B8" s="20" t="s">
@@ -3546,7 +3546,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="29.45" customHeight="1">
+    <row r="9" spans="1:10" ht="29.4" customHeight="1">
       <c r="B9" s="23" t="s">
         <v>23</v>
       </c>
@@ -3565,9 +3565,9 @@
       <c r="G9" s="24"/>
       <c r="H9" s="17"/>
       <c r="I9" s="27"/>
-      <c r="J9" s="77"/>
-    </row>
-    <row r="10" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J9" s="84"/>
+    </row>
+    <row r="10" spans="1:10" ht="13.95" customHeight="1">
       <c r="B10" s="25"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
@@ -3580,9 +3580,9 @@
       <c r="G10" s="24"/>
       <c r="H10" s="17"/>
       <c r="I10" s="17"/>
-      <c r="J10" s="75"/>
-    </row>
-    <row r="11" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J10" s="76"/>
+    </row>
+    <row r="11" spans="1:10" ht="13.95" customHeight="1">
       <c r="B11" s="25"/>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
@@ -3595,9 +3595,9 @@
       <c r="G11" s="24"/>
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
-      <c r="J11" s="75"/>
-    </row>
-    <row r="12" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J11" s="76"/>
+    </row>
+    <row r="12" spans="1:10" ht="13.95" customHeight="1">
       <c r="B12" s="25"/>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
@@ -3610,7 +3610,7 @@
       <c r="G12" s="24"/>
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
-      <c r="J12" s="75"/>
+      <c r="J12" s="76"/>
     </row>
     <row r="13" spans="1:10" ht="27" customHeight="1">
       <c r="B13" s="25"/>
@@ -3625,7 +3625,7 @@
       <c r="G13" s="24"/>
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
-      <c r="J13" s="75"/>
+      <c r="J13" s="76"/>
     </row>
     <row r="14" spans="1:10" ht="18" customHeight="1">
       <c r="B14" s="25"/>
@@ -3636,9 +3636,9 @@
       <c r="G14" s="24"/>
       <c r="H14" s="17"/>
       <c r="I14" s="17"/>
-      <c r="J14" s="78"/>
-    </row>
-    <row r="16" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J14" s="85"/>
+    </row>
+    <row r="16" spans="1:10" ht="13.95" customHeight="1">
       <c r="A16" s="18" t="s">
         <v>0</v>
       </c>
@@ -3704,9 +3704,9 @@
       <c r="G18" s="24"/>
       <c r="H18" s="17"/>
       <c r="I18" s="28"/>
-      <c r="J18" s="82"/>
-    </row>
-    <row r="19" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J18" s="80"/>
+    </row>
+    <row r="19" spans="1:10" ht="13.95" customHeight="1">
       <c r="B19" s="25"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -3719,9 +3719,9 @@
       <c r="G19" s="24"/>
       <c r="H19" s="17"/>
       <c r="I19" s="28"/>
-      <c r="J19" s="82"/>
-    </row>
-    <row r="20" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J19" s="80"/>
+    </row>
+    <row r="20" spans="1:10" ht="13.95" customHeight="1">
       <c r="B20" s="25"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
@@ -3732,9 +3732,9 @@
       <c r="G20" s="24"/>
       <c r="H20" s="17"/>
       <c r="I20" s="28"/>
-      <c r="J20" s="82"/>
-    </row>
-    <row r="21" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J20" s="80"/>
+    </row>
+    <row r="21" spans="1:10" ht="13.95" customHeight="1">
       <c r="B21" s="25"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
@@ -3747,9 +3747,9 @@
       <c r="G21" s="24"/>
       <c r="H21" s="17"/>
       <c r="I21" s="28"/>
-      <c r="J21" s="82"/>
-    </row>
-    <row r="22" spans="1:10" ht="28.15" customHeight="1">
+      <c r="J21" s="80"/>
+    </row>
+    <row r="22" spans="1:10" ht="28.2" customHeight="1">
       <c r="B22" s="25"/>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
@@ -3762,9 +3762,9 @@
       <c r="G22" s="24"/>
       <c r="H22" s="17"/>
       <c r="I22" s="28"/>
-      <c r="J22" s="82"/>
-    </row>
-    <row r="23" spans="1:10" ht="16.899999999999999" customHeight="1">
+      <c r="J22" s="80"/>
+    </row>
+    <row r="23" spans="1:10" ht="16.95" customHeight="1">
       <c r="B23" s="25"/>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
@@ -3773,12 +3773,12 @@
       <c r="G23" s="24"/>
       <c r="H23" s="17"/>
       <c r="I23" s="28"/>
-      <c r="J23" s="82"/>
+      <c r="J23" s="80"/>
     </row>
     <row r="24" spans="1:10">
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="1:10" ht="13.9" customHeight="1">
+    <row r="25" spans="1:10" ht="13.95" customHeight="1">
       <c r="A25" s="18" t="s">
         <v>0</v>
       </c>
@@ -3796,7 +3796,7 @@
       <c r="I25" s="51"/>
       <c r="J25" s="51"/>
     </row>
-    <row r="26" spans="1:10" ht="13.9" customHeight="1">
+    <row r="26" spans="1:10" ht="13.95" customHeight="1">
       <c r="B26" s="20" t="s">
         <v>1</v>
       </c>
@@ -3846,7 +3846,7 @@
       <c r="I27" s="17"/>
       <c r="J27" s="74"/>
     </row>
-    <row r="28" spans="1:10" ht="13.9" customHeight="1">
+    <row r="28" spans="1:10" ht="13.95" customHeight="1">
       <c r="B28" s="25"/>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
@@ -3859,9 +3859,9 @@
       <c r="G28" s="24"/>
       <c r="H28" s="17"/>
       <c r="I28" s="17"/>
-      <c r="J28" s="75"/>
-    </row>
-    <row r="29" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J28" s="76"/>
+    </row>
+    <row r="29" spans="1:10" ht="13.95" customHeight="1">
       <c r="B29" s="25"/>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
@@ -3874,9 +3874,9 @@
       <c r="G29" s="24"/>
       <c r="H29" s="17"/>
       <c r="I29" s="17"/>
-      <c r="J29" s="75"/>
-    </row>
-    <row r="30" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J29" s="76"/>
+    </row>
+    <row r="30" spans="1:10" ht="13.95" customHeight="1">
       <c r="B30" s="25"/>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
@@ -3887,9 +3887,9 @@
       <c r="G30" s="24"/>
       <c r="H30" s="17"/>
       <c r="I30" s="17"/>
-      <c r="J30" s="75"/>
-    </row>
-    <row r="31" spans="1:10" ht="28.9" customHeight="1">
+      <c r="J30" s="76"/>
+    </row>
+    <row r="31" spans="1:10" ht="28.95" customHeight="1">
       <c r="B31" s="25"/>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
@@ -3902,7 +3902,7 @@
       <c r="G31" s="24"/>
       <c r="H31" s="17"/>
       <c r="I31" s="17"/>
-      <c r="J31" s="75"/>
+      <c r="J31" s="76"/>
     </row>
     <row r="32" spans="1:10" ht="33" customHeight="1">
       <c r="B32" s="25"/>
@@ -3913,9 +3913,9 @@
       <c r="G32" s="24"/>
       <c r="H32" s="17"/>
       <c r="I32" s="17"/>
-      <c r="J32" s="76"/>
-    </row>
-    <row r="34" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J32" s="75"/>
+    </row>
+    <row r="34" spans="1:10" ht="13.95" customHeight="1">
       <c r="A34" s="18" t="s">
         <v>0</v>
       </c>
@@ -3933,7 +3933,7 @@
       <c r="I34" s="51"/>
       <c r="J34" s="51"/>
     </row>
-    <row r="35" spans="1:10" ht="25.15" customHeight="1">
+    <row r="35" spans="1:10" ht="25.2" customHeight="1">
       <c r="B35" s="20" t="s">
         <v>1</v>
       </c>
@@ -3962,7 +3962,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="25.15" customHeight="1">
+    <row r="36" spans="1:10" ht="25.2" customHeight="1">
       <c r="B36" s="23" t="s">
         <v>26</v>
       </c>
@@ -3983,7 +3983,7 @@
       <c r="I36" s="17"/>
       <c r="J36" s="74"/>
     </row>
-    <row r="37" spans="1:10" ht="13.9" customHeight="1">
+    <row r="37" spans="1:10" ht="13.95" customHeight="1">
       <c r="B37" s="25"/>
       <c r="C37" s="17"/>
       <c r="D37" s="17"/>
@@ -3996,9 +3996,9 @@
       <c r="G37" s="24"/>
       <c r="H37" s="17"/>
       <c r="I37" s="17"/>
-      <c r="J37" s="75"/>
-    </row>
-    <row r="38" spans="1:10" ht="16.149999999999999" customHeight="1">
+      <c r="J37" s="76"/>
+    </row>
+    <row r="38" spans="1:10" ht="16.2" customHeight="1">
       <c r="B38" s="25"/>
       <c r="C38" s="17"/>
       <c r="D38" s="17"/>
@@ -4011,9 +4011,9 @@
       <c r="G38" s="24"/>
       <c r="H38" s="17"/>
       <c r="I38" s="17"/>
-      <c r="J38" s="75"/>
-    </row>
-    <row r="39" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J38" s="76"/>
+    </row>
+    <row r="39" spans="1:10" ht="13.95" customHeight="1">
       <c r="B39" s="25"/>
       <c r="C39" s="17"/>
       <c r="D39" s="17"/>
@@ -4026,7 +4026,7 @@
       <c r="G39" s="24"/>
       <c r="H39" s="17"/>
       <c r="I39" s="17"/>
-      <c r="J39" s="75"/>
+      <c r="J39" s="76"/>
     </row>
     <row r="40" spans="1:10" ht="36" customHeight="1">
       <c r="B40" s="25"/>
@@ -4041,7 +4041,7 @@
       <c r="G40" s="24"/>
       <c r="H40" s="17"/>
       <c r="I40" s="17"/>
-      <c r="J40" s="75"/>
+      <c r="J40" s="76"/>
     </row>
     <row r="41" spans="1:10" ht="18" customHeight="1">
       <c r="B41" s="25"/>
@@ -4052,9 +4052,9 @@
       <c r="G41" s="17"/>
       <c r="H41" s="17"/>
       <c r="I41" s="17"/>
-      <c r="J41" s="76"/>
-    </row>
-    <row r="43" spans="1:10" ht="17.45" customHeight="1">
+      <c r="J41" s="75"/>
+    </row>
+    <row r="43" spans="1:10" ht="17.399999999999999" customHeight="1">
       <c r="A43" s="18" t="s">
         <v>0</v>
       </c>
@@ -4101,7 +4101,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="41.45" customHeight="1">
+    <row r="45" spans="1:10" ht="41.4" customHeight="1">
       <c r="B45" s="23" t="s">
         <v>28</v>
       </c>
@@ -4122,7 +4122,7 @@
       <c r="I45" s="17"/>
       <c r="J45" s="74"/>
     </row>
-    <row r="46" spans="1:10" ht="26.45" customHeight="1">
+    <row r="46" spans="1:10" ht="26.4" customHeight="1">
       <c r="B46" s="25"/>
       <c r="C46" s="17"/>
       <c r="D46" s="17"/>
@@ -4135,9 +4135,9 @@
       <c r="G46" s="24"/>
       <c r="H46" s="17"/>
       <c r="I46" s="17"/>
-      <c r="J46" s="75"/>
-    </row>
-    <row r="47" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J46" s="76"/>
+    </row>
+    <row r="47" spans="1:10" ht="13.95" customHeight="1">
       <c r="B47" s="25"/>
       <c r="C47" s="17"/>
       <c r="D47" s="17"/>
@@ -4150,9 +4150,9 @@
       <c r="G47" s="24"/>
       <c r="H47" s="17"/>
       <c r="I47" s="17"/>
-      <c r="J47" s="75"/>
-    </row>
-    <row r="48" spans="1:10" ht="25.9" customHeight="1">
+      <c r="J47" s="76"/>
+    </row>
+    <row r="48" spans="1:10" ht="25.95" customHeight="1">
       <c r="B48" s="25"/>
       <c r="C48" s="17"/>
       <c r="D48" s="17"/>
@@ -4165,9 +4165,9 @@
       <c r="G48" s="24"/>
       <c r="H48" s="17"/>
       <c r="I48" s="17"/>
-      <c r="J48" s="75"/>
-    </row>
-    <row r="49" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J48" s="76"/>
+    </row>
+    <row r="49" spans="1:10" ht="13.95" customHeight="1">
       <c r="B49" s="25"/>
       <c r="C49" s="17"/>
       <c r="D49" s="17"/>
@@ -4176,9 +4176,9 @@
       <c r="G49" s="17"/>
       <c r="H49" s="17"/>
       <c r="I49" s="17"/>
-      <c r="J49" s="76"/>
-    </row>
-    <row r="51" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J49" s="75"/>
+    </row>
+    <row r="51" spans="1:10" ht="13.95" customHeight="1">
       <c r="A51" s="18" t="s">
         <v>0</v>
       </c>
@@ -4196,7 +4196,7 @@
       <c r="I51" s="51"/>
       <c r="J51" s="51"/>
     </row>
-    <row r="52" spans="1:10" ht="13.9" customHeight="1">
+    <row r="52" spans="1:10" ht="13.95" customHeight="1">
       <c r="B52" s="20" t="s">
         <v>1</v>
       </c>
@@ -4225,7 +4225,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="25.15" customHeight="1">
+    <row r="53" spans="1:10" ht="25.2" customHeight="1">
       <c r="B53" s="23" t="s">
         <v>30</v>
       </c>
@@ -4246,7 +4246,7 @@
       <c r="I53" s="17"/>
       <c r="J53" s="74"/>
     </row>
-    <row r="54" spans="1:10" ht="26.45" customHeight="1">
+    <row r="54" spans="1:10" ht="26.4" customHeight="1">
       <c r="B54" s="25"/>
       <c r="C54" s="17"/>
       <c r="D54" s="17"/>
@@ -4259,9 +4259,9 @@
       <c r="G54" s="24"/>
       <c r="H54" s="17"/>
       <c r="I54" s="17"/>
-      <c r="J54" s="75"/>
-    </row>
-    <row r="55" spans="1:10" ht="29.45" customHeight="1">
+      <c r="J54" s="76"/>
+    </row>
+    <row r="55" spans="1:10" ht="29.4" customHeight="1">
       <c r="B55" s="25"/>
       <c r="C55" s="17"/>
       <c r="D55" s="17"/>
@@ -4274,9 +4274,9 @@
       <c r="G55" s="24"/>
       <c r="H55" s="17"/>
       <c r="I55" s="17"/>
-      <c r="J55" s="75"/>
-    </row>
-    <row r="56" spans="1:10" ht="28.15" customHeight="1">
+      <c r="J55" s="76"/>
+    </row>
+    <row r="56" spans="1:10" ht="28.2" customHeight="1">
       <c r="B56" s="25"/>
       <c r="C56" s="17"/>
       <c r="D56" s="17"/>
@@ -4285,9 +4285,9 @@
       <c r="G56" s="24"/>
       <c r="H56" s="17"/>
       <c r="I56" s="17"/>
-      <c r="J56" s="75"/>
-    </row>
-    <row r="58" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J56" s="76"/>
+    </row>
+    <row r="58" spans="1:10" ht="13.95" customHeight="1">
       <c r="A58" s="18" t="s">
         <v>0</v>
       </c>
@@ -4305,7 +4305,7 @@
       <c r="I58" s="61"/>
       <c r="J58" s="62"/>
     </row>
-    <row r="59" spans="1:10" ht="13.9" customHeight="1">
+    <row r="59" spans="1:10" ht="13.95" customHeight="1">
       <c r="B59" s="20" t="s">
         <v>1</v>
       </c>
@@ -4334,7 +4334,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="40.15" customHeight="1">
+    <row r="60" spans="1:10" ht="40.200000000000003" customHeight="1">
       <c r="B60" s="23" t="s">
         <v>39</v>
       </c>
@@ -4355,7 +4355,7 @@
       <c r="I60" s="17"/>
       <c r="J60" s="74"/>
     </row>
-    <row r="61" spans="1:10" ht="13.9" customHeight="1">
+    <row r="61" spans="1:10" ht="13.95" customHeight="1">
       <c r="B61" s="25"/>
       <c r="C61" s="17"/>
       <c r="D61" s="17"/>
@@ -4368,9 +4368,9 @@
       <c r="G61" s="24"/>
       <c r="H61" s="17"/>
       <c r="I61" s="17"/>
-      <c r="J61" s="75"/>
-    </row>
-    <row r="62" spans="1:10" ht="28.9" customHeight="1">
+      <c r="J61" s="76"/>
+    </row>
+    <row r="62" spans="1:10" ht="28.95" customHeight="1">
       <c r="B62" s="25"/>
       <c r="C62" s="17"/>
       <c r="D62" s="17"/>
@@ -4383,9 +4383,9 @@
       <c r="G62" s="24"/>
       <c r="H62" s="17"/>
       <c r="I62" s="17"/>
-      <c r="J62" s="75"/>
-    </row>
-    <row r="63" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J62" s="76"/>
+    </row>
+    <row r="63" spans="1:10" ht="13.95" customHeight="1">
       <c r="B63" s="25"/>
       <c r="C63" s="17"/>
       <c r="D63" s="17"/>
@@ -4398,7 +4398,7 @@
       <c r="G63" s="24"/>
       <c r="H63" s="17"/>
       <c r="I63" s="17"/>
-      <c r="J63" s="75"/>
+      <c r="J63" s="76"/>
     </row>
     <row r="64" spans="1:10" ht="45.6" customHeight="1">
       <c r="B64" s="25"/>
@@ -4413,9 +4413,9 @@
       <c r="G64" s="24"/>
       <c r="H64" s="17"/>
       <c r="I64" s="17"/>
-      <c r="J64" s="75"/>
-    </row>
-    <row r="65" spans="1:10" ht="17.45" customHeight="1">
+      <c r="J64" s="76"/>
+    </row>
+    <row r="65" spans="1:10" ht="17.399999999999999" customHeight="1">
       <c r="B65" s="25"/>
       <c r="C65" s="17"/>
       <c r="D65" s="17"/>
@@ -4424,9 +4424,9 @@
       <c r="G65" s="17"/>
       <c r="H65" s="17"/>
       <c r="I65" s="17"/>
-      <c r="J65" s="76"/>
-    </row>
-    <row r="67" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J65" s="75"/>
+    </row>
+    <row r="67" spans="1:10" ht="13.95" customHeight="1">
       <c r="A67" s="18" t="s">
         <v>0</v>
       </c>
@@ -4444,7 +4444,7 @@
       <c r="I67" s="51"/>
       <c r="J67" s="51"/>
     </row>
-    <row r="68" spans="1:10" ht="13.9" customHeight="1">
+    <row r="68" spans="1:10" ht="13.95" customHeight="1">
       <c r="B68" s="20" t="s">
         <v>1</v>
       </c>
@@ -4494,7 +4494,7 @@
       <c r="I69" s="17"/>
       <c r="J69" s="74"/>
     </row>
-    <row r="70" spans="1:10" ht="13.9" customHeight="1">
+    <row r="70" spans="1:10" ht="13.95" customHeight="1">
       <c r="B70" s="25"/>
       <c r="C70" s="17"/>
       <c r="D70" s="17"/>
@@ -4507,9 +4507,9 @@
       <c r="G70" s="24"/>
       <c r="H70" s="17"/>
       <c r="I70" s="17"/>
-      <c r="J70" s="75"/>
-    </row>
-    <row r="71" spans="1:10" ht="16.899999999999999" customHeight="1">
+      <c r="J70" s="76"/>
+    </row>
+    <row r="71" spans="1:10" ht="16.95" customHeight="1">
       <c r="B71" s="25"/>
       <c r="C71" s="17"/>
       <c r="D71" s="17"/>
@@ -4522,7 +4522,7 @@
       <c r="G71" s="24"/>
       <c r="H71" s="17"/>
       <c r="I71" s="17"/>
-      <c r="J71" s="75"/>
+      <c r="J71" s="76"/>
     </row>
     <row r="72" spans="1:10" ht="30.6" customHeight="1">
       <c r="B72" s="25"/>
@@ -4537,9 +4537,9 @@
       <c r="G72" s="24"/>
       <c r="H72" s="17"/>
       <c r="I72" s="17"/>
-      <c r="J72" s="75"/>
-    </row>
-    <row r="73" spans="1:10" ht="38.450000000000003" customHeight="1">
+      <c r="J72" s="76"/>
+    </row>
+    <row r="73" spans="1:10" ht="38.4" customHeight="1">
       <c r="B73" s="25"/>
       <c r="C73" s="17"/>
       <c r="D73" s="17"/>
@@ -4552,7 +4552,7 @@
       <c r="G73" s="24"/>
       <c r="H73" s="17"/>
       <c r="I73" s="17"/>
-      <c r="J73" s="75"/>
+      <c r="J73" s="76"/>
     </row>
     <row r="74" spans="1:10" ht="27" customHeight="1">
       <c r="B74" s="25"/>
@@ -4563,9 +4563,9 @@
       <c r="G74" s="24"/>
       <c r="H74" s="17"/>
       <c r="I74" s="17"/>
-      <c r="J74" s="76"/>
-    </row>
-    <row r="76" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J74" s="75"/>
+    </row>
+    <row r="76" spans="1:10" ht="13.95" customHeight="1">
       <c r="A76" s="18" t="s">
         <v>0</v>
       </c>
@@ -4583,7 +4583,7 @@
       <c r="I76" s="51"/>
       <c r="J76" s="51"/>
     </row>
-    <row r="77" spans="1:10" ht="13.9" customHeight="1">
+    <row r="77" spans="1:10" ht="13.95" customHeight="1">
       <c r="B77" s="20" t="s">
         <v>1</v>
       </c>
@@ -4612,7 +4612,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="25.15" customHeight="1">
+    <row r="78" spans="1:10" ht="25.2" customHeight="1">
       <c r="B78" s="23" t="s">
         <v>35</v>
       </c>
@@ -4633,7 +4633,7 @@
       <c r="I78" s="17"/>
       <c r="J78" s="74"/>
     </row>
-    <row r="79" spans="1:10" ht="13.9" customHeight="1">
+    <row r="79" spans="1:10" ht="13.95" customHeight="1">
       <c r="B79" s="25"/>
       <c r="C79" s="17"/>
       <c r="D79" s="17"/>
@@ -4646,9 +4646,9 @@
       <c r="G79" s="24"/>
       <c r="H79" s="17"/>
       <c r="I79" s="17"/>
-      <c r="J79" s="75"/>
-    </row>
-    <row r="80" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J79" s="76"/>
+    </row>
+    <row r="80" spans="1:10" ht="13.95" customHeight="1">
       <c r="B80" s="25"/>
       <c r="C80" s="17"/>
       <c r="D80" s="17"/>
@@ -4659,7 +4659,7 @@
       <c r="G80" s="24"/>
       <c r="H80" s="17"/>
       <c r="I80" s="17"/>
-      <c r="J80" s="75"/>
+      <c r="J80" s="76"/>
     </row>
     <row r="81" spans="1:10" ht="45" customHeight="1">
       <c r="B81" s="25"/>
@@ -4674,7 +4674,7 @@
       <c r="G81" s="24"/>
       <c r="H81" s="17"/>
       <c r="I81" s="17"/>
-      <c r="J81" s="75"/>
+      <c r="J81" s="76"/>
     </row>
     <row r="82" spans="1:10" ht="18.600000000000001" customHeight="1">
       <c r="B82" s="25"/>
@@ -4685,7 +4685,7 @@
       <c r="G82" s="17"/>
       <c r="H82" s="17"/>
       <c r="I82" s="17"/>
-      <c r="J82" s="76"/>
+      <c r="J82" s="75"/>
     </row>
     <row r="83" spans="1:10" ht="18.600000000000001" customHeight="1">
       <c r="B83" s="42"/>
@@ -4710,7 +4710,7 @@
       <c r="I84" s="47"/>
       <c r="J84" s="48"/>
     </row>
-    <row r="86" spans="1:10" ht="13.9" customHeight="1">
+    <row r="86" spans="1:10" ht="13.95" customHeight="1">
       <c r="A86" s="18" t="s">
         <v>0</v>
       </c>
@@ -4728,7 +4728,7 @@
       <c r="I86" s="51"/>
       <c r="J86" s="51"/>
     </row>
-    <row r="87" spans="1:10" ht="13.9" customHeight="1">
+    <row r="87" spans="1:10" ht="13.95" customHeight="1">
       <c r="B87" s="20" t="s">
         <v>1</v>
       </c>
@@ -4778,7 +4778,7 @@
       <c r="I88" s="17"/>
       <c r="J88" s="74"/>
     </row>
-    <row r="89" spans="1:10" ht="29.45" customHeight="1">
+    <row r="89" spans="1:10" ht="29.4" customHeight="1">
       <c r="B89" s="25"/>
       <c r="C89" s="17"/>
       <c r="D89" s="17"/>
@@ -4791,9 +4791,9 @@
       <c r="G89" s="24"/>
       <c r="H89" s="17"/>
       <c r="I89" s="17"/>
-      <c r="J89" s="75"/>
-    </row>
-    <row r="90" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J89" s="76"/>
+    </row>
+    <row r="90" spans="1:10" ht="13.95" customHeight="1">
       <c r="B90" s="25"/>
       <c r="C90" s="17"/>
       <c r="D90" s="17"/>
@@ -4806,9 +4806,9 @@
       <c r="G90" s="24"/>
       <c r="H90" s="17"/>
       <c r="I90" s="17"/>
-      <c r="J90" s="75"/>
-    </row>
-    <row r="91" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J90" s="76"/>
+    </row>
+    <row r="91" spans="1:10" ht="13.95" customHeight="1">
       <c r="B91" s="25"/>
       <c r="C91" s="17"/>
       <c r="D91" s="17"/>
@@ -4821,9 +4821,9 @@
       <c r="G91" s="24"/>
       <c r="H91" s="17"/>
       <c r="I91" s="17"/>
-      <c r="J91" s="75"/>
-    </row>
-    <row r="92" spans="1:10" ht="53.45" customHeight="1">
+      <c r="J91" s="76"/>
+    </row>
+    <row r="92" spans="1:10" ht="53.4" customHeight="1">
       <c r="B92" s="25"/>
       <c r="C92" s="17"/>
       <c r="D92" s="17"/>
@@ -4836,7 +4836,7 @@
       <c r="G92" s="24"/>
       <c r="H92" s="17"/>
       <c r="I92" s="17"/>
-      <c r="J92" s="75"/>
+      <c r="J92" s="76"/>
     </row>
     <row r="93" spans="1:10" ht="18" customHeight="1">
       <c r="B93" s="25"/>
@@ -4847,9 +4847,9 @@
       <c r="G93" s="24"/>
       <c r="H93" s="17"/>
       <c r="I93" s="17"/>
-      <c r="J93" s="76"/>
-    </row>
-    <row r="95" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J93" s="75"/>
+    </row>
+    <row r="95" spans="1:10" ht="13.95" customHeight="1">
       <c r="A95" s="18" t="s">
         <v>0</v>
       </c>
@@ -4867,7 +4867,7 @@
       <c r="I95" s="51"/>
       <c r="J95" s="51"/>
     </row>
-    <row r="96" spans="1:10" ht="13.9" customHeight="1">
+    <row r="96" spans="1:10" ht="13.95" customHeight="1">
       <c r="B96" s="20" t="s">
         <v>1</v>
       </c>
@@ -4896,7 +4896,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="40.9" customHeight="1">
+    <row r="97" spans="1:10" ht="40.950000000000003" customHeight="1">
       <c r="B97" s="23" t="s">
         <v>35</v>
       </c>
@@ -4917,7 +4917,7 @@
       <c r="I97" s="17"/>
       <c r="J97" s="74"/>
     </row>
-    <row r="98" spans="1:10" ht="13.9" customHeight="1">
+    <row r="98" spans="1:10" ht="13.95" customHeight="1">
       <c r="B98" s="25"/>
       <c r="C98" s="17"/>
       <c r="D98" s="17"/>
@@ -4928,9 +4928,9 @@
       <c r="G98" s="24"/>
       <c r="H98" s="17"/>
       <c r="I98" s="17"/>
-      <c r="J98" s="75"/>
-    </row>
-    <row r="99" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J98" s="76"/>
+    </row>
+    <row r="99" spans="1:10" ht="13.95" customHeight="1">
       <c r="B99" s="25"/>
       <c r="C99" s="17"/>
       <c r="D99" s="17"/>
@@ -4943,9 +4943,9 @@
       <c r="G99" s="24"/>
       <c r="H99" s="17"/>
       <c r="I99" s="17"/>
-      <c r="J99" s="75"/>
-    </row>
-    <row r="100" spans="1:10" ht="20.45" customHeight="1">
+      <c r="J99" s="76"/>
+    </row>
+    <row r="100" spans="1:10" ht="20.399999999999999" customHeight="1">
       <c r="B100" s="25"/>
       <c r="C100" s="17"/>
       <c r="D100" s="17"/>
@@ -4958,9 +4958,9 @@
       <c r="G100" s="24"/>
       <c r="H100" s="17"/>
       <c r="I100" s="17"/>
-      <c r="J100" s="75"/>
-    </row>
-    <row r="101" spans="1:10" ht="40.15" customHeight="1">
+      <c r="J100" s="76"/>
+    </row>
+    <row r="101" spans="1:10" ht="40.200000000000003" customHeight="1">
       <c r="B101" s="25"/>
       <c r="C101" s="17"/>
       <c r="D101" s="17"/>
@@ -4973,7 +4973,7 @@
       <c r="G101" s="24"/>
       <c r="H101" s="17"/>
       <c r="I101" s="17"/>
-      <c r="J101" s="75"/>
+      <c r="J101" s="76"/>
     </row>
     <row r="102" spans="1:10" ht="27.6" customHeight="1">
       <c r="B102" s="25"/>
@@ -4984,9 +4984,9 @@
       <c r="G102" s="24"/>
       <c r="H102" s="17"/>
       <c r="I102" s="17"/>
-      <c r="J102" s="76"/>
-    </row>
-    <row r="104" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J102" s="75"/>
+    </row>
+    <row r="104" spans="1:10" ht="13.95" customHeight="1">
       <c r="A104" s="18" t="s">
         <v>0</v>
       </c>
@@ -5004,7 +5004,7 @@
       <c r="I104" s="51"/>
       <c r="J104" s="51"/>
     </row>
-    <row r="105" spans="1:10" ht="13.9" customHeight="1">
+    <row r="105" spans="1:10" ht="13.95" customHeight="1">
       <c r="B105" s="20" t="s">
         <v>1</v>
       </c>
@@ -5033,7 +5033,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="40.9" customHeight="1">
+    <row r="106" spans="1:10" ht="40.950000000000003" customHeight="1">
       <c r="B106" s="23" t="s">
         <v>36</v>
       </c>
@@ -5067,9 +5067,9 @@
       <c r="G107" s="24"/>
       <c r="H107" s="17"/>
       <c r="I107" s="17"/>
-      <c r="J107" s="75"/>
-    </row>
-    <row r="108" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J107" s="76"/>
+    </row>
+    <row r="108" spans="1:10" ht="13.95" customHeight="1">
       <c r="B108" s="25"/>
       <c r="C108" s="17"/>
       <c r="D108" s="17"/>
@@ -5082,9 +5082,9 @@
       <c r="G108" s="24"/>
       <c r="H108" s="17"/>
       <c r="I108" s="17"/>
-      <c r="J108" s="75"/>
-    </row>
-    <row r="109" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J108" s="76"/>
+    </row>
+    <row r="109" spans="1:10" ht="13.95" customHeight="1">
       <c r="B109" s="25"/>
       <c r="C109" s="17"/>
       <c r="D109" s="17"/>
@@ -5097,9 +5097,9 @@
       <c r="G109" s="24"/>
       <c r="H109" s="17"/>
       <c r="I109" s="17"/>
-      <c r="J109" s="75"/>
-    </row>
-    <row r="110" spans="1:10" ht="43.15" customHeight="1">
+      <c r="J109" s="76"/>
+    </row>
+    <row r="110" spans="1:10" ht="43.2" customHeight="1">
       <c r="B110" s="25"/>
       <c r="C110" s="17"/>
       <c r="D110" s="17"/>
@@ -5112,7 +5112,7 @@
       <c r="G110" s="24"/>
       <c r="H110" s="17"/>
       <c r="I110" s="17"/>
-      <c r="J110" s="75"/>
+      <c r="J110" s="76"/>
     </row>
     <row r="111" spans="1:10" ht="27.6" customHeight="1">
       <c r="B111" s="25"/>
@@ -5123,9 +5123,9 @@
       <c r="G111" s="24"/>
       <c r="H111" s="17"/>
       <c r="I111" s="17"/>
-      <c r="J111" s="76"/>
-    </row>
-    <row r="113" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J111" s="75"/>
+    </row>
+    <row r="113" spans="1:10" ht="13.95" customHeight="1">
       <c r="A113" s="18" t="s">
         <v>0</v>
       </c>
@@ -5143,7 +5143,7 @@
       <c r="I113" s="51"/>
       <c r="J113" s="51"/>
     </row>
-    <row r="114" spans="1:10" ht="13.9" customHeight="1">
+    <row r="114" spans="1:10" ht="13.95" customHeight="1">
       <c r="B114" s="20" t="s">
         <v>1</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="40.9" customHeight="1">
+    <row r="115" spans="1:10" ht="40.950000000000003" customHeight="1">
       <c r="B115" s="23" t="s">
         <v>37</v>
       </c>
@@ -5206,9 +5206,9 @@
       <c r="G116" s="24"/>
       <c r="H116" s="17"/>
       <c r="I116" s="17"/>
-      <c r="J116" s="75"/>
-    </row>
-    <row r="117" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J116" s="76"/>
+    </row>
+    <row r="117" spans="1:10" ht="13.95" customHeight="1">
       <c r="B117" s="25"/>
       <c r="C117" s="17"/>
       <c r="D117" s="17"/>
@@ -5221,9 +5221,9 @@
       <c r="G117" s="24"/>
       <c r="H117" s="17"/>
       <c r="I117" s="17"/>
-      <c r="J117" s="75"/>
-    </row>
-    <row r="118" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J117" s="76"/>
+    </row>
+    <row r="118" spans="1:10" ht="13.95" customHeight="1">
       <c r="B118" s="25"/>
       <c r="C118" s="17"/>
       <c r="D118" s="17"/>
@@ -5236,9 +5236,9 @@
       <c r="G118" s="24"/>
       <c r="H118" s="17"/>
       <c r="I118" s="17"/>
-      <c r="J118" s="75"/>
-    </row>
-    <row r="119" spans="1:10" ht="40.15" customHeight="1">
+      <c r="J118" s="76"/>
+    </row>
+    <row r="119" spans="1:10" ht="40.200000000000003" customHeight="1">
       <c r="B119" s="25"/>
       <c r="C119" s="17"/>
       <c r="D119" s="17"/>
@@ -5251,7 +5251,7 @@
       <c r="G119" s="24"/>
       <c r="H119" s="17"/>
       <c r="I119" s="17"/>
-      <c r="J119" s="75"/>
+      <c r="J119" s="76"/>
     </row>
     <row r="120" spans="1:10" ht="27.6" customHeight="1">
       <c r="B120" s="25"/>
@@ -5262,9 +5262,9 @@
       <c r="G120" s="24"/>
       <c r="H120" s="17"/>
       <c r="I120" s="17"/>
-      <c r="J120" s="76"/>
-    </row>
-    <row r="122" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J120" s="75"/>
+    </row>
+    <row r="122" spans="1:10" ht="13.95" customHeight="1">
       <c r="A122" s="18" t="s">
         <v>0</v>
       </c>
@@ -5282,7 +5282,7 @@
       <c r="I122" s="51"/>
       <c r="J122" s="51"/>
     </row>
-    <row r="123" spans="1:10" ht="13.9" customHeight="1">
+    <row r="123" spans="1:10" ht="13.95" customHeight="1">
       <c r="B123" s="20" t="s">
         <v>1</v>
       </c>
@@ -5311,7 +5311,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="124" spans="1:10" ht="40.9" customHeight="1">
+    <row r="124" spans="1:10" ht="40.950000000000003" customHeight="1">
       <c r="B124" s="23" t="s">
         <v>53</v>
       </c>
@@ -5332,7 +5332,7 @@
       <c r="I124" s="17"/>
       <c r="J124" s="74"/>
     </row>
-    <row r="125" spans="1:10" ht="17.45" customHeight="1">
+    <row r="125" spans="1:10" ht="17.399999999999999" customHeight="1">
       <c r="B125" s="25"/>
       <c r="C125" s="17"/>
       <c r="D125" s="17"/>
@@ -5345,9 +5345,9 @@
       <c r="G125" s="24"/>
       <c r="H125" s="17"/>
       <c r="I125" s="17"/>
-      <c r="J125" s="75"/>
-    </row>
-    <row r="126" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J125" s="76"/>
+    </row>
+    <row r="126" spans="1:10" ht="13.95" customHeight="1">
       <c r="B126" s="25"/>
       <c r="C126" s="17"/>
       <c r="D126" s="17"/>
@@ -5360,9 +5360,9 @@
       <c r="G126" s="24"/>
       <c r="H126" s="17"/>
       <c r="I126" s="17"/>
-      <c r="J126" s="75"/>
-    </row>
-    <row r="127" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J126" s="76"/>
+    </row>
+    <row r="127" spans="1:10" ht="13.95" customHeight="1">
       <c r="B127" s="25"/>
       <c r="C127" s="17"/>
       <c r="D127" s="17"/>
@@ -5373,9 +5373,9 @@
       <c r="G127" s="24"/>
       <c r="H127" s="17"/>
       <c r="I127" s="17"/>
-      <c r="J127" s="75"/>
-    </row>
-    <row r="128" spans="1:10" ht="40.9" customHeight="1">
+      <c r="J127" s="76"/>
+    </row>
+    <row r="128" spans="1:10" ht="40.950000000000003" customHeight="1">
       <c r="B128" s="25"/>
       <c r="C128" s="17"/>
       <c r="D128" s="17"/>
@@ -5388,7 +5388,7 @@
       <c r="G128" s="24"/>
       <c r="H128" s="17"/>
       <c r="I128" s="17"/>
-      <c r="J128" s="75"/>
+      <c r="J128" s="76"/>
     </row>
     <row r="129" spans="1:10" ht="27.6" customHeight="1">
       <c r="B129" s="25"/>
@@ -5399,9 +5399,9 @@
       <c r="G129" s="24"/>
       <c r="H129" s="17"/>
       <c r="I129" s="17"/>
-      <c r="J129" s="76"/>
-    </row>
-    <row r="131" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J129" s="75"/>
+    </row>
+    <row r="131" spans="1:10" ht="13.95" customHeight="1">
       <c r="A131" s="18" t="s">
         <v>0</v>
       </c>
@@ -5419,7 +5419,7 @@
       <c r="I131" s="51"/>
       <c r="J131" s="51"/>
     </row>
-    <row r="132" spans="1:10" ht="13.9" customHeight="1">
+    <row r="132" spans="1:10" ht="13.95" customHeight="1">
       <c r="B132" s="20" t="s">
         <v>1</v>
       </c>
@@ -5448,7 +5448,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="133" spans="1:10" ht="51">
+    <row r="133" spans="1:10" ht="52.8">
       <c r="B133" s="23" t="s">
         <v>56</v>
       </c>
@@ -5469,7 +5469,7 @@
       <c r="I133" s="17"/>
       <c r="J133" s="74"/>
     </row>
-    <row r="134" spans="1:10" ht="13.9" customHeight="1">
+    <row r="134" spans="1:10" ht="13.95" customHeight="1">
       <c r="B134" s="25"/>
       <c r="C134" s="17"/>
       <c r="D134" s="17"/>
@@ -5482,9 +5482,9 @@
       <c r="G134" s="24"/>
       <c r="H134" s="17"/>
       <c r="I134" s="17"/>
-      <c r="J134" s="75"/>
-    </row>
-    <row r="135" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J134" s="76"/>
+    </row>
+    <row r="135" spans="1:10" ht="13.95" customHeight="1">
       <c r="B135" s="25"/>
       <c r="C135" s="17"/>
       <c r="D135" s="17"/>
@@ -5497,7 +5497,7 @@
       <c r="G135" s="24"/>
       <c r="H135" s="17"/>
       <c r="I135" s="17"/>
-      <c r="J135" s="75"/>
+      <c r="J135" s="76"/>
     </row>
     <row r="136" spans="1:10" ht="30" customHeight="1">
       <c r="B136" s="25"/>
@@ -5512,9 +5512,9 @@
       <c r="G136" s="24"/>
       <c r="H136" s="17"/>
       <c r="I136" s="17"/>
-      <c r="J136" s="75"/>
-    </row>
-    <row r="137" spans="1:10" ht="40.15" customHeight="1">
+      <c r="J136" s="76"/>
+    </row>
+    <row r="137" spans="1:10" ht="40.200000000000003" customHeight="1">
       <c r="B137" s="25"/>
       <c r="C137" s="17"/>
       <c r="D137" s="17"/>
@@ -5527,7 +5527,7 @@
       <c r="G137" s="24"/>
       <c r="H137" s="17"/>
       <c r="I137" s="17"/>
-      <c r="J137" s="75"/>
+      <c r="J137" s="76"/>
     </row>
     <row r="138" spans="1:10" ht="27.6" customHeight="1">
       <c r="B138" s="25"/>
@@ -5538,9 +5538,9 @@
       <c r="G138" s="24"/>
       <c r="H138" s="17"/>
       <c r="I138" s="17"/>
-      <c r="J138" s="76"/>
-    </row>
-    <row r="140" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J138" s="75"/>
+    </row>
+    <row r="140" spans="1:10" ht="13.95" customHeight="1">
       <c r="A140" s="18" t="s">
         <v>0</v>
       </c>
@@ -5558,7 +5558,7 @@
       <c r="I140" s="51"/>
       <c r="J140" s="51"/>
     </row>
-    <row r="141" spans="1:10" ht="13.9" customHeight="1">
+    <row r="141" spans="1:10" ht="13.95" customHeight="1">
       <c r="B141" s="20" t="s">
         <v>1</v>
       </c>
@@ -5587,7 +5587,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="142" spans="1:10" ht="40.9" customHeight="1">
+    <row r="142" spans="1:10" ht="40.950000000000003" customHeight="1">
       <c r="B142" s="23" t="s">
         <v>62</v>
       </c>
@@ -5608,7 +5608,7 @@
       <c r="I142" s="17"/>
       <c r="J142" s="74"/>
     </row>
-    <row r="143" spans="1:10" ht="13.9" customHeight="1">
+    <row r="143" spans="1:10" ht="13.95" customHeight="1">
       <c r="B143" s="25"/>
       <c r="C143" s="17"/>
       <c r="D143" s="17"/>
@@ -5621,9 +5621,9 @@
       <c r="G143" s="24"/>
       <c r="H143" s="17"/>
       <c r="I143" s="17"/>
-      <c r="J143" s="75"/>
-    </row>
-    <row r="144" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J143" s="76"/>
+    </row>
+    <row r="144" spans="1:10" ht="13.95" customHeight="1">
       <c r="B144" s="25"/>
       <c r="C144" s="17"/>
       <c r="D144" s="17"/>
@@ -5634,7 +5634,7 @@
       <c r="G144" s="24"/>
       <c r="H144" s="17"/>
       <c r="I144" s="17"/>
-      <c r="J144" s="75"/>
+      <c r="J144" s="76"/>
     </row>
     <row r="145" spans="1:10" ht="15.6" customHeight="1">
       <c r="B145" s="25"/>
@@ -5649,9 +5649,9 @@
       <c r="G145" s="24"/>
       <c r="H145" s="17"/>
       <c r="I145" s="17"/>
-      <c r="J145" s="75"/>
-    </row>
-    <row r="146" spans="1:10" ht="34.9" customHeight="1">
+      <c r="J145" s="76"/>
+    </row>
+    <row r="146" spans="1:10" ht="34.950000000000003" customHeight="1">
       <c r="B146" s="25"/>
       <c r="C146" s="17"/>
       <c r="D146" s="17"/>
@@ -5664,7 +5664,7 @@
       <c r="G146" s="24"/>
       <c r="H146" s="17"/>
       <c r="I146" s="17"/>
-      <c r="J146" s="75"/>
+      <c r="J146" s="76"/>
     </row>
     <row r="147" spans="1:10" ht="27.6" customHeight="1">
       <c r="B147" s="25"/>
@@ -5675,9 +5675,9 @@
       <c r="G147" s="24"/>
       <c r="H147" s="17"/>
       <c r="I147" s="17"/>
-      <c r="J147" s="76"/>
-    </row>
-    <row r="149" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J147" s="75"/>
+    </row>
+    <row r="149" spans="1:10" ht="13.95" customHeight="1">
       <c r="A149" s="18" t="s">
         <v>0</v>
       </c>
@@ -5695,7 +5695,7 @@
       <c r="I149" s="51"/>
       <c r="J149" s="51"/>
     </row>
-    <row r="150" spans="1:10" ht="13.9" customHeight="1">
+    <row r="150" spans="1:10" ht="13.95" customHeight="1">
       <c r="B150" s="20" t="s">
         <v>1</v>
       </c>
@@ -5724,7 +5724,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="151" spans="1:10" ht="40.9" customHeight="1">
+    <row r="151" spans="1:10" ht="40.950000000000003" customHeight="1">
       <c r="B151" s="23" t="s">
         <v>64</v>
       </c>
@@ -5745,7 +5745,7 @@
       <c r="I151" s="17"/>
       <c r="J151" s="74"/>
     </row>
-    <row r="152" spans="1:10" ht="13.9" customHeight="1">
+    <row r="152" spans="1:10" ht="13.95" customHeight="1">
       <c r="B152" s="25"/>
       <c r="C152" s="17"/>
       <c r="D152" s="17"/>
@@ -5758,9 +5758,9 @@
       <c r="G152" s="24"/>
       <c r="H152" s="17"/>
       <c r="I152" s="17"/>
-      <c r="J152" s="75"/>
-    </row>
-    <row r="153" spans="1:10" ht="29.45" customHeight="1">
+      <c r="J152" s="76"/>
+    </row>
+    <row r="153" spans="1:10" ht="29.4" customHeight="1">
       <c r="B153" s="25"/>
       <c r="C153" s="17"/>
       <c r="D153" s="17"/>
@@ -5773,9 +5773,9 @@
       <c r="G153" s="24"/>
       <c r="H153" s="17"/>
       <c r="I153" s="17"/>
-      <c r="J153" s="75"/>
-    </row>
-    <row r="154" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J153" s="76"/>
+    </row>
+    <row r="154" spans="1:10" ht="13.95" customHeight="1">
       <c r="B154" s="25"/>
       <c r="C154" s="17"/>
       <c r="D154" s="17"/>
@@ -5788,7 +5788,7 @@
       <c r="G154" s="24"/>
       <c r="H154" s="17"/>
       <c r="I154" s="17"/>
-      <c r="J154" s="75"/>
+      <c r="J154" s="76"/>
     </row>
     <row r="155" spans="1:10" ht="30" customHeight="1">
       <c r="B155" s="25"/>
@@ -5803,7 +5803,7 @@
       <c r="G155" s="24"/>
       <c r="H155" s="17"/>
       <c r="I155" s="17"/>
-      <c r="J155" s="75"/>
+      <c r="J155" s="76"/>
     </row>
     <row r="156" spans="1:10" ht="27.6" customHeight="1">
       <c r="B156" s="25"/>
@@ -5814,9 +5814,9 @@
       <c r="G156" s="24"/>
       <c r="H156" s="17"/>
       <c r="I156" s="17"/>
-      <c r="J156" s="76"/>
-    </row>
-    <row r="158" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J156" s="75"/>
+    </row>
+    <row r="158" spans="1:10" ht="13.95" customHeight="1">
       <c r="A158" s="18" t="s">
         <v>0</v>
       </c>
@@ -5834,7 +5834,7 @@
       <c r="I158" s="51"/>
       <c r="J158" s="51"/>
     </row>
-    <row r="159" spans="1:10" ht="13.9" customHeight="1">
+    <row r="159" spans="1:10" ht="13.95" customHeight="1">
       <c r="B159" s="20" t="s">
         <v>1</v>
       </c>
@@ -5863,7 +5863,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="160" spans="1:10" ht="40.9" customHeight="1">
+    <row r="160" spans="1:10" ht="40.950000000000003" customHeight="1">
       <c r="B160" s="23" t="s">
         <v>67</v>
       </c>
@@ -5884,7 +5884,7 @@
       <c r="I160" s="17"/>
       <c r="J160" s="74"/>
     </row>
-    <row r="161" spans="1:10" ht="13.9" customHeight="1">
+    <row r="161" spans="1:10" ht="13.95" customHeight="1">
       <c r="B161" s="25"/>
       <c r="C161" s="17"/>
       <c r="D161" s="17"/>
@@ -5897,7 +5897,7 @@
       <c r="G161" s="24"/>
       <c r="H161" s="17"/>
       <c r="I161" s="17"/>
-      <c r="J161" s="75"/>
+      <c r="J161" s="76"/>
     </row>
     <row r="162" spans="1:10" ht="27.6" customHeight="1">
       <c r="B162" s="25"/>
@@ -5912,9 +5912,9 @@
       <c r="G162" s="24"/>
       <c r="H162" s="17"/>
       <c r="I162" s="17"/>
-      <c r="J162" s="75"/>
-    </row>
-    <row r="163" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J162" s="76"/>
+    </row>
+    <row r="163" spans="1:10" ht="13.95" customHeight="1">
       <c r="B163" s="25"/>
       <c r="C163" s="17"/>
       <c r="D163" s="17"/>
@@ -5927,7 +5927,7 @@
       <c r="G163" s="24"/>
       <c r="H163" s="17"/>
       <c r="I163" s="17"/>
-      <c r="J163" s="75"/>
+      <c r="J163" s="76"/>
     </row>
     <row r="164" spans="1:10" ht="30" customHeight="1">
       <c r="B164" s="25"/>
@@ -5942,7 +5942,7 @@
       <c r="G164" s="24"/>
       <c r="H164" s="17"/>
       <c r="I164" s="17"/>
-      <c r="J164" s="75"/>
+      <c r="J164" s="76"/>
     </row>
     <row r="165" spans="1:10" ht="27.6" customHeight="1">
       <c r="B165" s="25"/>
@@ -5953,9 +5953,9 @@
       <c r="G165" s="24"/>
       <c r="H165" s="17"/>
       <c r="I165" s="17"/>
-      <c r="J165" s="76"/>
-    </row>
-    <row r="167" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J165" s="75"/>
+    </row>
+    <row r="167" spans="1:10" ht="13.95" customHeight="1">
       <c r="A167" s="18" t="s">
         <v>0</v>
       </c>
@@ -5973,7 +5973,7 @@
       <c r="I167" s="51"/>
       <c r="J167" s="51"/>
     </row>
-    <row r="168" spans="1:10" ht="13.9" customHeight="1">
+    <row r="168" spans="1:10" ht="13.95" customHeight="1">
       <c r="B168" s="20" t="s">
         <v>1</v>
       </c>
@@ -6002,7 +6002,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="169" spans="1:10" ht="40.9" customHeight="1">
+    <row r="169" spans="1:10" ht="40.950000000000003" customHeight="1">
       <c r="B169" s="23" t="s">
         <v>68</v>
       </c>
@@ -6023,7 +6023,7 @@
       <c r="I169" s="17"/>
       <c r="J169" s="74"/>
     </row>
-    <row r="170" spans="1:10" ht="26.45" customHeight="1">
+    <row r="170" spans="1:10" ht="26.4" customHeight="1">
       <c r="B170" s="25"/>
       <c r="C170" s="17"/>
       <c r="D170" s="17"/>
@@ -6036,7 +6036,7 @@
       <c r="G170" s="24"/>
       <c r="H170" s="17"/>
       <c r="I170" s="17"/>
-      <c r="J170" s="75"/>
+      <c r="J170" s="76"/>
     </row>
     <row r="171" spans="1:10" ht="27.6" customHeight="1">
       <c r="B171" s="25"/>
@@ -6047,9 +6047,9 @@
       <c r="G171" s="24"/>
       <c r="H171" s="17"/>
       <c r="I171" s="17"/>
-      <c r="J171" s="76"/>
-    </row>
-    <row r="173" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J171" s="75"/>
+    </row>
+    <row r="173" spans="1:10" ht="13.95" customHeight="1">
       <c r="A173" s="18" t="s">
         <v>0</v>
       </c>
@@ -6067,7 +6067,7 @@
       <c r="I173" s="51"/>
       <c r="J173" s="51"/>
     </row>
-    <row r="174" spans="1:10" ht="13.9" customHeight="1">
+    <row r="174" spans="1:10" ht="13.95" customHeight="1">
       <c r="B174" s="20" t="s">
         <v>1</v>
       </c>
@@ -6096,7 +6096,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="175" spans="1:10" ht="40.9" customHeight="1">
+    <row r="175" spans="1:10" ht="40.950000000000003" customHeight="1">
       <c r="B175" s="23" t="s">
         <v>71</v>
       </c>
@@ -6130,9 +6130,9 @@
       <c r="G176" s="24"/>
       <c r="H176" s="17"/>
       <c r="I176" s="17"/>
-      <c r="J176" s="75"/>
-    </row>
-    <row r="177" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J176" s="76"/>
+    </row>
+    <row r="177" spans="1:10" ht="13.95" customHeight="1">
       <c r="B177" s="25"/>
       <c r="C177" s="17"/>
       <c r="D177" s="17"/>
@@ -6145,9 +6145,9 @@
       <c r="G177" s="24"/>
       <c r="H177" s="17"/>
       <c r="I177" s="17"/>
-      <c r="J177" s="75"/>
-    </row>
-    <row r="178" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J177" s="76"/>
+    </row>
+    <row r="178" spans="1:10" ht="13.95" customHeight="1">
       <c r="B178" s="25"/>
       <c r="C178" s="17"/>
       <c r="D178" s="17"/>
@@ -6160,9 +6160,9 @@
       <c r="G178" s="24"/>
       <c r="H178" s="17"/>
       <c r="I178" s="17"/>
-      <c r="J178" s="75"/>
-    </row>
-    <row r="179" spans="1:10" ht="19.899999999999999" customHeight="1">
+      <c r="J178" s="76"/>
+    </row>
+    <row r="179" spans="1:10" ht="19.95" customHeight="1">
       <c r="B179" s="25"/>
       <c r="C179" s="17"/>
       <c r="D179" s="17"/>
@@ -6175,7 +6175,7 @@
       <c r="G179" s="24"/>
       <c r="H179" s="17"/>
       <c r="I179" s="17"/>
-      <c r="J179" s="75"/>
+      <c r="J179" s="76"/>
     </row>
     <row r="180" spans="1:10" ht="27.6" customHeight="1">
       <c r="B180" s="25"/>
@@ -6190,9 +6190,9 @@
       <c r="G180" s="24"/>
       <c r="H180" s="17"/>
       <c r="I180" s="17"/>
-      <c r="J180" s="76"/>
-    </row>
-    <row r="182" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J180" s="75"/>
+    </row>
+    <row r="182" spans="1:10" ht="13.95" customHeight="1">
       <c r="A182" s="18" t="s">
         <v>0</v>
       </c>
@@ -6210,7 +6210,7 @@
       <c r="I182" s="51"/>
       <c r="J182" s="51"/>
     </row>
-    <row r="183" spans="1:10" ht="13.9" customHeight="1">
+    <row r="183" spans="1:10" ht="13.95" customHeight="1">
       <c r="B183" s="20" t="s">
         <v>1</v>
       </c>
@@ -6239,7 +6239,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:10" ht="40.9" customHeight="1">
+    <row r="184" spans="1:10" ht="40.950000000000003" customHeight="1">
       <c r="B184" s="23" t="s">
         <v>72</v>
       </c>
@@ -6260,7 +6260,7 @@
       <c r="I184" s="17"/>
       <c r="J184" s="74"/>
     </row>
-    <row r="185" spans="1:10" ht="13.9" customHeight="1">
+    <row r="185" spans="1:10" ht="13.95" customHeight="1">
       <c r="B185" s="25"/>
       <c r="C185" s="17"/>
       <c r="D185" s="17"/>
@@ -6273,9 +6273,9 @@
       <c r="G185" s="24"/>
       <c r="H185" s="17"/>
       <c r="I185" s="17"/>
-      <c r="J185" s="75"/>
-    </row>
-    <row r="186" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J185" s="76"/>
+    </row>
+    <row r="186" spans="1:10" ht="13.95" customHeight="1">
       <c r="B186" s="25"/>
       <c r="C186" s="17"/>
       <c r="D186" s="17"/>
@@ -6288,9 +6288,9 @@
       <c r="G186" s="24"/>
       <c r="H186" s="17"/>
       <c r="I186" s="17"/>
-      <c r="J186" s="75"/>
-    </row>
-    <row r="187" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J186" s="76"/>
+    </row>
+    <row r="187" spans="1:10" ht="13.95" customHeight="1">
       <c r="B187" s="25"/>
       <c r="C187" s="17"/>
       <c r="D187" s="17"/>
@@ -6303,9 +6303,9 @@
       <c r="G187" s="24"/>
       <c r="H187" s="17"/>
       <c r="I187" s="17"/>
-      <c r="J187" s="75"/>
-    </row>
-    <row r="188" spans="1:10" ht="37.9" customHeight="1">
+      <c r="J187" s="76"/>
+    </row>
+    <row r="188" spans="1:10" ht="37.950000000000003" customHeight="1">
       <c r="B188" s="25"/>
       <c r="C188" s="17"/>
       <c r="D188" s="17"/>
@@ -6318,7 +6318,7 @@
       <c r="G188" s="24"/>
       <c r="H188" s="17"/>
       <c r="I188" s="17"/>
-      <c r="J188" s="75"/>
+      <c r="J188" s="76"/>
     </row>
     <row r="189" spans="1:10" ht="54" customHeight="1">
       <c r="B189" s="25"/>
@@ -6335,9 +6335,9 @@
       <c r="G189" s="24"/>
       <c r="H189" s="17"/>
       <c r="I189" s="17"/>
-      <c r="J189" s="75"/>
-    </row>
-    <row r="190" spans="1:10" ht="25.9" customHeight="1">
+      <c r="J189" s="76"/>
+    </row>
+    <row r="190" spans="1:10" ht="25.95" customHeight="1">
       <c r="B190" s="25"/>
       <c r="C190" s="17"/>
       <c r="D190" s="17"/>
@@ -6350,9 +6350,9 @@
       <c r="G190" s="24"/>
       <c r="H190" s="17"/>
       <c r="I190" s="17"/>
-      <c r="J190" s="75"/>
-    </row>
-    <row r="191" spans="1:10" ht="31.15" customHeight="1">
+      <c r="J190" s="76"/>
+    </row>
+    <row r="191" spans="1:10" ht="31.2" customHeight="1">
       <c r="B191" s="25"/>
       <c r="C191" s="17"/>
       <c r="D191" s="17"/>
@@ -6365,9 +6365,9 @@
       <c r="G191" s="24"/>
       <c r="H191" s="17"/>
       <c r="I191" s="17"/>
-      <c r="J191" s="75"/>
-    </row>
-    <row r="192" spans="1:10" ht="29.45" customHeight="1">
+      <c r="J191" s="76"/>
+    </row>
+    <row r="192" spans="1:10" ht="29.4" customHeight="1">
       <c r="B192" s="25"/>
       <c r="C192" s="17"/>
       <c r="D192" s="17"/>
@@ -6380,7 +6380,7 @@
       <c r="G192" s="24"/>
       <c r="H192" s="17"/>
       <c r="I192" s="17"/>
-      <c r="J192" s="75"/>
+      <c r="J192" s="76"/>
     </row>
     <row r="193" spans="1:10" ht="42" customHeight="1">
       <c r="B193" s="25"/>
@@ -6395,7 +6395,7 @@
       <c r="G193" s="24"/>
       <c r="H193" s="17"/>
       <c r="I193" s="17"/>
-      <c r="J193" s="75"/>
+      <c r="J193" s="76"/>
     </row>
     <row r="194" spans="1:10" ht="15.6" customHeight="1">
       <c r="B194" s="25"/>
@@ -6406,9 +6406,9 @@
       <c r="G194" s="24"/>
       <c r="H194" s="17"/>
       <c r="I194" s="17"/>
-      <c r="J194" s="76"/>
-    </row>
-    <row r="196" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J194" s="75"/>
+    </row>
+    <row r="196" spans="1:10" ht="13.95" customHeight="1">
       <c r="A196" s="18" t="s">
         <v>0</v>
       </c>
@@ -6426,7 +6426,7 @@
       <c r="I196" s="51"/>
       <c r="J196" s="51"/>
     </row>
-    <row r="197" spans="1:10" ht="13.9" customHeight="1">
+    <row r="197" spans="1:10" ht="13.95" customHeight="1">
       <c r="B197" s="20" t="s">
         <v>1</v>
       </c>
@@ -6455,7 +6455,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="198" spans="1:10" ht="40.9" customHeight="1">
+    <row r="198" spans="1:10" ht="40.950000000000003" customHeight="1">
       <c r="B198" s="23" t="s">
         <v>75</v>
       </c>
@@ -6476,7 +6476,7 @@
       <c r="I198" s="17"/>
       <c r="J198" s="74"/>
     </row>
-    <row r="199" spans="1:10" ht="13.9" customHeight="1">
+    <row r="199" spans="1:10" ht="13.95" customHeight="1">
       <c r="B199" s="25"/>
       <c r="C199" s="17"/>
       <c r="D199" s="17"/>
@@ -6487,9 +6487,9 @@
       <c r="G199" s="24"/>
       <c r="H199" s="17"/>
       <c r="I199" s="17"/>
-      <c r="J199" s="75"/>
-    </row>
-    <row r="200" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J199" s="76"/>
+    </row>
+    <row r="200" spans="1:10" ht="13.95" customHeight="1">
       <c r="B200" s="25"/>
       <c r="C200" s="17"/>
       <c r="D200" s="17"/>
@@ -6500,9 +6500,9 @@
       <c r="G200" s="24"/>
       <c r="H200" s="17"/>
       <c r="I200" s="17"/>
-      <c r="J200" s="75"/>
-    </row>
-    <row r="201" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J200" s="76"/>
+    </row>
+    <row r="201" spans="1:10" ht="13.95" customHeight="1">
       <c r="B201" s="25"/>
       <c r="C201" s="17"/>
       <c r="D201" s="17"/>
@@ -6513,7 +6513,7 @@
       <c r="G201" s="24"/>
       <c r="H201" s="17"/>
       <c r="I201" s="17"/>
-      <c r="J201" s="75"/>
+      <c r="J201" s="76"/>
     </row>
     <row r="202" spans="1:10" ht="42.6" customHeight="1">
       <c r="B202" s="25"/>
@@ -6528,7 +6528,7 @@
       <c r="G202" s="24"/>
       <c r="H202" s="17"/>
       <c r="I202" s="17"/>
-      <c r="J202" s="75"/>
+      <c r="J202" s="76"/>
     </row>
     <row r="203" spans="1:10" ht="27.6" customHeight="1">
       <c r="B203" s="25"/>
@@ -6539,9 +6539,9 @@
       <c r="G203" s="24"/>
       <c r="H203" s="17"/>
       <c r="I203" s="17"/>
-      <c r="J203" s="76"/>
-    </row>
-    <row r="205" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J203" s="75"/>
+    </row>
+    <row r="205" spans="1:10" ht="13.95" customHeight="1">
       <c r="A205" s="18" t="s">
         <v>0</v>
       </c>
@@ -6559,7 +6559,7 @@
       <c r="I205" s="51"/>
       <c r="J205" s="51"/>
     </row>
-    <row r="206" spans="1:10" ht="13.9" customHeight="1">
+    <row r="206" spans="1:10" ht="13.95" customHeight="1">
       <c r="B206" s="20" t="s">
         <v>1</v>
       </c>
@@ -6588,7 +6588,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="207" spans="1:10" ht="40.9" customHeight="1">
+    <row r="207" spans="1:10" ht="40.950000000000003" customHeight="1">
       <c r="B207" s="23" t="s">
         <v>77</v>
       </c>
@@ -6609,7 +6609,7 @@
       <c r="I207" s="17"/>
       <c r="J207" s="74"/>
     </row>
-    <row r="208" spans="1:10" ht="13.9" customHeight="1">
+    <row r="208" spans="1:10" ht="13.95" customHeight="1">
       <c r="B208" s="25"/>
       <c r="C208" s="17"/>
       <c r="D208" s="17"/>
@@ -6622,9 +6622,9 @@
       <c r="G208" s="24"/>
       <c r="H208" s="17"/>
       <c r="I208" s="17"/>
-      <c r="J208" s="75"/>
-    </row>
-    <row r="209" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J208" s="76"/>
+    </row>
+    <row r="209" spans="1:10" ht="13.95" customHeight="1">
       <c r="B209" s="25"/>
       <c r="C209" s="17"/>
       <c r="D209" s="17"/>
@@ -6637,9 +6637,9 @@
       <c r="G209" s="24"/>
       <c r="H209" s="17"/>
       <c r="I209" s="17"/>
-      <c r="J209" s="75"/>
-    </row>
-    <row r="210" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J209" s="76"/>
+    </row>
+    <row r="210" spans="1:10" ht="13.95" customHeight="1">
       <c r="B210" s="25"/>
       <c r="C210" s="17"/>
       <c r="D210" s="17"/>
@@ -6652,9 +6652,9 @@
       <c r="G210" s="24"/>
       <c r="H210" s="17"/>
       <c r="I210" s="17"/>
-      <c r="J210" s="75"/>
-    </row>
-    <row r="211" spans="1:10" ht="28.15" customHeight="1">
+      <c r="J210" s="76"/>
+    </row>
+    <row r="211" spans="1:10" ht="28.2" customHeight="1">
       <c r="B211" s="25"/>
       <c r="C211" s="17"/>
       <c r="D211" s="17"/>
@@ -6667,9 +6667,9 @@
       <c r="G211" s="24"/>
       <c r="H211" s="17"/>
       <c r="I211" s="17"/>
-      <c r="J211" s="75"/>
-    </row>
-    <row r="212" spans="1:10" ht="28.9" customHeight="1">
+      <c r="J211" s="76"/>
+    </row>
+    <row r="212" spans="1:10" ht="28.95" customHeight="1">
       <c r="B212" s="25"/>
       <c r="C212" s="17"/>
       <c r="D212" s="17"/>
@@ -6682,9 +6682,9 @@
       <c r="G212" s="24"/>
       <c r="H212" s="17"/>
       <c r="I212" s="17"/>
-      <c r="J212" s="75"/>
-    </row>
-    <row r="213" spans="1:10" ht="14.45" customHeight="1">
+      <c r="J212" s="76"/>
+    </row>
+    <row r="213" spans="1:10" ht="14.4" customHeight="1">
       <c r="B213" s="25"/>
       <c r="C213" s="17"/>
       <c r="D213" s="17"/>
@@ -6693,9 +6693,9 @@
       <c r="G213" s="24"/>
       <c r="H213" s="17"/>
       <c r="I213" s="17"/>
-      <c r="J213" s="76"/>
-    </row>
-    <row r="215" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J213" s="75"/>
+    </row>
+    <row r="215" spans="1:10" ht="13.95" customHeight="1">
       <c r="A215" s="18" t="s">
         <v>0</v>
       </c>
@@ -6713,7 +6713,7 @@
       <c r="I215" s="51"/>
       <c r="J215" s="51"/>
     </row>
-    <row r="216" spans="1:10" ht="13.9" customHeight="1">
+    <row r="216" spans="1:10" ht="13.95" customHeight="1">
       <c r="B216" s="20" t="s">
         <v>1</v>
       </c>
@@ -6742,7 +6742,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="217" spans="1:10" ht="40.9" customHeight="1">
+    <row r="217" spans="1:10" ht="40.950000000000003" customHeight="1">
       <c r="B217" s="23" t="s">
         <v>78</v>
       </c>
@@ -6763,7 +6763,7 @@
       <c r="I217" s="17"/>
       <c r="J217" s="74"/>
     </row>
-    <row r="218" spans="1:10" ht="13.9" customHeight="1">
+    <row r="218" spans="1:10" ht="13.95" customHeight="1">
       <c r="B218" s="25"/>
       <c r="C218" s="17"/>
       <c r="D218" s="17"/>
@@ -6776,9 +6776,9 @@
       <c r="G218" s="24"/>
       <c r="H218" s="17"/>
       <c r="I218" s="17"/>
-      <c r="J218" s="75"/>
-    </row>
-    <row r="219" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J218" s="76"/>
+    </row>
+    <row r="219" spans="1:10" ht="13.95" customHeight="1">
       <c r="B219" s="25"/>
       <c r="C219" s="17"/>
       <c r="D219" s="17"/>
@@ -6791,9 +6791,9 @@
       <c r="G219" s="24"/>
       <c r="H219" s="17"/>
       <c r="I219" s="17"/>
-      <c r="J219" s="75"/>
-    </row>
-    <row r="220" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J219" s="76"/>
+    </row>
+    <row r="220" spans="1:10" ht="13.95" customHeight="1">
       <c r="B220" s="25"/>
       <c r="C220" s="17"/>
       <c r="D220" s="17"/>
@@ -6806,7 +6806,7 @@
       <c r="G220" s="24"/>
       <c r="H220" s="17"/>
       <c r="I220" s="17"/>
-      <c r="J220" s="75"/>
+      <c r="J220" s="76"/>
     </row>
     <row r="221" spans="1:10" ht="30" customHeight="1">
       <c r="B221" s="25"/>
@@ -6821,7 +6821,7 @@
       <c r="G221" s="24"/>
       <c r="H221" s="17"/>
       <c r="I221" s="17"/>
-      <c r="J221" s="75"/>
+      <c r="J221" s="76"/>
     </row>
     <row r="222" spans="1:10" ht="27.6" customHeight="1">
       <c r="B222" s="25"/>
@@ -6836,9 +6836,9 @@
       <c r="G222" s="24"/>
       <c r="H222" s="17"/>
       <c r="I222" s="17"/>
-      <c r="J222" s="76"/>
-    </row>
-    <row r="224" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J222" s="75"/>
+    </row>
+    <row r="224" spans="1:10" ht="13.95" customHeight="1">
       <c r="A224" s="18" t="s">
         <v>0</v>
       </c>
@@ -6856,7 +6856,7 @@
       <c r="I224" s="51"/>
       <c r="J224" s="51"/>
     </row>
-    <row r="225" spans="1:10" ht="13.9" customHeight="1">
+    <row r="225" spans="1:10" ht="13.95" customHeight="1">
       <c r="B225" s="20" t="s">
         <v>1</v>
       </c>
@@ -6885,7 +6885,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="226" spans="1:10" ht="40.9" customHeight="1">
+    <row r="226" spans="1:10" ht="40.950000000000003" customHeight="1">
       <c r="B226" s="23" t="s">
         <v>86</v>
       </c>
@@ -6906,7 +6906,7 @@
       <c r="I226" s="17"/>
       <c r="J226" s="74"/>
     </row>
-    <row r="227" spans="1:10" ht="13.9" customHeight="1">
+    <row r="227" spans="1:10" ht="13.95" customHeight="1">
       <c r="B227" s="25"/>
       <c r="C227" s="17"/>
       <c r="D227" s="17"/>
@@ -6919,9 +6919,9 @@
       <c r="G227" s="24"/>
       <c r="H227" s="17"/>
       <c r="I227" s="17"/>
-      <c r="J227" s="75"/>
-    </row>
-    <row r="228" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J227" s="76"/>
+    </row>
+    <row r="228" spans="1:10" ht="13.95" customHeight="1">
       <c r="B228" s="25"/>
       <c r="C228" s="17"/>
       <c r="D228" s="17"/>
@@ -6934,9 +6934,9 @@
       <c r="G228" s="24"/>
       <c r="H228" s="17"/>
       <c r="I228" s="17"/>
-      <c r="J228" s="75"/>
-    </row>
-    <row r="229" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J228" s="76"/>
+    </row>
+    <row r="229" spans="1:10" ht="13.95" customHeight="1">
       <c r="B229" s="25"/>
       <c r="C229" s="17"/>
       <c r="D229" s="17"/>
@@ -6949,7 +6949,7 @@
       <c r="G229" s="24"/>
       <c r="H229" s="17"/>
       <c r="I229" s="17"/>
-      <c r="J229" s="75"/>
+      <c r="J229" s="76"/>
     </row>
     <row r="230" spans="1:10" ht="30" customHeight="1">
       <c r="B230" s="25"/>
@@ -6964,7 +6964,7 @@
       <c r="G230" s="24"/>
       <c r="H230" s="17"/>
       <c r="I230" s="17"/>
-      <c r="J230" s="75"/>
+      <c r="J230" s="76"/>
     </row>
     <row r="231" spans="1:10" ht="27.6" customHeight="1">
       <c r="B231" s="25"/>
@@ -6979,9 +6979,9 @@
       <c r="G231" s="24"/>
       <c r="H231" s="17"/>
       <c r="I231" s="17"/>
-      <c r="J231" s="76"/>
-    </row>
-    <row r="233" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J231" s="75"/>
+    </row>
+    <row r="233" spans="1:10" ht="13.95" customHeight="1">
       <c r="A233" s="18" t="s">
         <v>0</v>
       </c>
@@ -6999,7 +6999,7 @@
       <c r="I233" s="51"/>
       <c r="J233" s="51"/>
     </row>
-    <row r="234" spans="1:10" ht="13.9" customHeight="1">
+    <row r="234" spans="1:10" ht="13.95" customHeight="1">
       <c r="B234" s="20" t="s">
         <v>1</v>
       </c>
@@ -7028,7 +7028,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="235" spans="1:10" ht="40.9" customHeight="1">
+    <row r="235" spans="1:10" ht="40.950000000000003" customHeight="1">
       <c r="B235" s="23" t="s">
         <v>92</v>
       </c>
@@ -7062,7 +7062,7 @@
       <c r="G236" s="24"/>
       <c r="H236" s="17"/>
       <c r="I236" s="17"/>
-      <c r="J236" s="75"/>
+      <c r="J236" s="76"/>
     </row>
     <row r="237" spans="1:10" ht="27.6" customHeight="1">
       <c r="B237" s="25"/>
@@ -7073,9 +7073,9 @@
       <c r="G237" s="24"/>
       <c r="H237" s="17"/>
       <c r="I237" s="17"/>
-      <c r="J237" s="76"/>
-    </row>
-    <row r="239" spans="1:10" ht="13.9" customHeight="1">
+      <c r="J237" s="75"/>
+    </row>
+    <row r="239" spans="1:10" ht="13.95" customHeight="1">
       <c r="A239" s="18" t="s">
         <v>0</v>
       </c>
@@ -7093,7 +7093,7 @@
       <c r="I239" s="51"/>
       <c r="J239" s="51"/>
     </row>
-    <row r="240" spans="1:10" ht="13.9" customHeight="1">
+    <row r="240" spans="1:10" ht="13.95" customHeight="1">
       <c r="B240" s="20" t="s">
         <v>1</v>
       </c>
@@ -7122,7 +7122,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="241" spans="2:10" ht="40.9" customHeight="1">
+    <row r="241" spans="2:10" ht="40.950000000000003" customHeight="1">
       <c r="B241" s="23" t="s">
         <v>107</v>
       </c>
@@ -7152,42 +7152,17 @@
       <c r="G242" s="24"/>
       <c r="H242" s="17"/>
       <c r="I242" s="17"/>
-      <c r="J242" s="76"/>
+      <c r="J242" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="C239:J239"/>
-    <mergeCell ref="J241:J242"/>
-    <mergeCell ref="J217:J222"/>
-    <mergeCell ref="C224:J224"/>
-    <mergeCell ref="J226:J231"/>
-    <mergeCell ref="C233:J233"/>
-    <mergeCell ref="J235:J237"/>
-    <mergeCell ref="C196:J196"/>
-    <mergeCell ref="J198:J203"/>
-    <mergeCell ref="C205:J205"/>
-    <mergeCell ref="J207:J213"/>
-    <mergeCell ref="C215:J215"/>
-    <mergeCell ref="J169:J171"/>
-    <mergeCell ref="C173:J173"/>
-    <mergeCell ref="J175:J180"/>
-    <mergeCell ref="C182:J182"/>
-    <mergeCell ref="J184:J194"/>
-    <mergeCell ref="C149:J149"/>
-    <mergeCell ref="J151:J156"/>
-    <mergeCell ref="C158:J158"/>
-    <mergeCell ref="J160:J165"/>
-    <mergeCell ref="C167:J167"/>
-    <mergeCell ref="J124:J129"/>
-    <mergeCell ref="C131:J131"/>
-    <mergeCell ref="J133:J138"/>
-    <mergeCell ref="C140:J140"/>
-    <mergeCell ref="J142:J147"/>
-    <mergeCell ref="C104:J104"/>
-    <mergeCell ref="J106:J111"/>
-    <mergeCell ref="C113:J113"/>
-    <mergeCell ref="J115:J120"/>
-    <mergeCell ref="C122:J122"/>
+    <mergeCell ref="J88:J93"/>
+    <mergeCell ref="J97:J102"/>
+    <mergeCell ref="C43:J43"/>
+    <mergeCell ref="J9:J14"/>
+    <mergeCell ref="J60:J65"/>
+    <mergeCell ref="J69:J74"/>
+    <mergeCell ref="J78:J82"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="J27:J32"/>
     <mergeCell ref="C86:J86"/>
@@ -7204,13 +7179,38 @@
     <mergeCell ref="C16:J16"/>
     <mergeCell ref="C25:J25"/>
     <mergeCell ref="C34:J34"/>
-    <mergeCell ref="J88:J93"/>
-    <mergeCell ref="J97:J102"/>
-    <mergeCell ref="C43:J43"/>
-    <mergeCell ref="J9:J14"/>
-    <mergeCell ref="J60:J65"/>
-    <mergeCell ref="J69:J74"/>
-    <mergeCell ref="J78:J82"/>
+    <mergeCell ref="C104:J104"/>
+    <mergeCell ref="J106:J111"/>
+    <mergeCell ref="C113:J113"/>
+    <mergeCell ref="J115:J120"/>
+    <mergeCell ref="C122:J122"/>
+    <mergeCell ref="J124:J129"/>
+    <mergeCell ref="C131:J131"/>
+    <mergeCell ref="J133:J138"/>
+    <mergeCell ref="C140:J140"/>
+    <mergeCell ref="J142:J147"/>
+    <mergeCell ref="C149:J149"/>
+    <mergeCell ref="J151:J156"/>
+    <mergeCell ref="C158:J158"/>
+    <mergeCell ref="J160:J165"/>
+    <mergeCell ref="C167:J167"/>
+    <mergeCell ref="J169:J171"/>
+    <mergeCell ref="C173:J173"/>
+    <mergeCell ref="J175:J180"/>
+    <mergeCell ref="C182:J182"/>
+    <mergeCell ref="J184:J194"/>
+    <mergeCell ref="C196:J196"/>
+    <mergeCell ref="J198:J203"/>
+    <mergeCell ref="C205:J205"/>
+    <mergeCell ref="J207:J213"/>
+    <mergeCell ref="C215:J215"/>
+    <mergeCell ref="C239:J239"/>
+    <mergeCell ref="J241:J242"/>
+    <mergeCell ref="J217:J222"/>
+    <mergeCell ref="C224:J224"/>
+    <mergeCell ref="J226:J231"/>
+    <mergeCell ref="C233:J233"/>
+    <mergeCell ref="J235:J237"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>